<commit_message>
feat: update proj battleworld to f9d77d5e07fe252dfc9d762178172fb58c738f56
</commit_message>
<xml_diff>
--- a/battleworld/Excel/MotionClip_技能数据.xlsx
+++ b/battleworld/Excel/MotionClip_技能数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,7 +534,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "21a9", "guid": "117383", "duration": 6, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "968e", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 17, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6d67", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 18, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "ccd5", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2000, "groundFriction": 1, "gravityScale": 1, "gravityTime": 0}], "1": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0f2e", "guid": "168948", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 0.8, "y": 1, "z": 0.8}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}], "2": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "462e", "breakType": 1}], "3": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "21a9", "guid": "117383", "duration": 6, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "968e", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 17, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6d67", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 18, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "ccd5", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2000, "groundFriction": 0, "gravityScale": 1, "gravityTime": 0}], "1": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0f2e", "guid": "168948", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 0.8, "y": 1, "z": 0.8}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}], "2": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "462e", "breakType": 1}], "3": []}</t>
         </is>
       </c>
     </row>
@@ -603,7 +603,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0223", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 18, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "0888", "guid": "151007", "duration": 12, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a82b", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 17, "colorHex": "", "colorHex1": ""}], "1": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3cf6", "guid": "168948", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 0.8, "y": 1, "z": 0.8}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Move", "frameGuid": "ca66", "move_offsetPos": {"x": 25, "y": 0, "z": 0}, "move_isFlash": 1, "move_count": 15}], "2": [], "3": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0223", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 18, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "0888", "guid": "151007", "duration": 12, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a82b", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 17, "colorHex": "", "colorHex1": ""}], "1": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3cf6", "guid": "168948", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 0.8, "y": 1, "z": 0.8}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Move", "frameGuid": "ca66", "move_offsetPos": {"x": 10, "y": 0, "z": 0}, "move_isFlash": 1, "move_count": 15}], "2": [], "3": []}</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0223", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 18, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "0888", "guid": "151008", "duration": 12, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a82b", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 17, "colorHex": "", "colorHex1": ""}], "1": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3cf6", "guid": "168948", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 0.8, "y": 1, "z": 0.8}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Move", "frameGuid": "ca66", "move_offsetPos": {"x": 25, "y": 0, "z": 0}, "move_isFlash": 1, "move_count": 15}], "2": [], "3": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0223", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 18, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "0888", "guid": "151008", "duration": 12, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a82b", "guid": "151528", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -4, "slotIndex": 17, "colorHex": "", "colorHex1": ""}], "1": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3cf6", "guid": "168948", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 0.8, "y": 1, "z": 0.8}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Move", "frameGuid": "ca66", "move_offsetPos": {"x": 10, "y": 0, "z": 0}, "move_isFlash": 1, "move_count": 15}], "2": [], "3": []}</t>
         </is>
       </c>
     </row>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>技能1</t>
+          <t>烈焰突刺</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>技能2</t>
+          <t>旋风斩击</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1745,7 +1745,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>技能3</t>
+          <t>爆炎重击</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>技能4</t>
+          <t>火雨</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1791,7 +1791,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>技能5</t>
+          <t>烈焰飞劈</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>技能6</t>
+          <t>巨焰剑气</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>技能7</t>
+          <t>巨焰竖斩</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>技能8</t>
+          <t>飞凰突击</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>技能9</t>
+          <t>火焰庇护</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>技能10</t>
+          <t>焰能觉醒</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1915,6 +1915,328 @@
       <c r="E65" t="inlineStr">
         <is>
           <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "c7b4", "guid": "121905", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "347d", "guid": "162431", "offsetPos": {"x": 30, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF4300FF"}], "2": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a600", "guid": "163348", "offsetPos": {"x": 75, "y": 0, "z": 42}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "16a8", "guid": "163348", "offsetPos": {"x": 75, "y": 0, "z": 42}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "3": [], "4": [], "5": [], "9": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "0f88", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5095", "guid": "151573", "offsetPos": {"x": 75, "y": 0, "z": 42}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF6A00FF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "37c9", "type": 1, "offsetLoc": {"x": 75, "y": 0, "z": -38}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 80, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "08a3", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 79, "dilationRate": 0, "dilationFrame": 0}], "12": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "3109", "breakType": 2}], "13": [], "16": []}</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>62</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>拳头普攻</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>怒气普攻1</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>14</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "211a", "guid": "122528", "duration": 15, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "e88a", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "2": [], "3": [], "4": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "845a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5a0d", "guid": "27702", "offsetPos": {"x": 100, "y": 6, "z": 10}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a028", "guid": "27702", "offsetPos": {"x": 100, "y": 6, "z": 10}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ff69", "guid": "51211", "offsetPos": {"x": 105, "y": 0, "z": 15}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 1.6, "y": 1.6, "z": 1.6}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1aab", "guid": "151566", "offsetPos": {"x": 100, "y": 0, "z": 10}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "ea41", "type": 1, "offsetLoc": {"x": 155, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 2.5, "y": 2.5, "z": 2.5}, "range": 3, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 1, "dilationRate": 0, "dilationFrame": 0}], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5854", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 0.02, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "6": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "bdfe", "breakType": 2}], "7": [], "8": [], "9": [], "10": [], "12": []}</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>63</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>拳头普攻</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>怒气普攻2</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>12</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "58f2", "guid": "122530", "duration": 14, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "9cfc", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "1": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "cac6", "offsetPos": {"x": -100, "y": 0, "z": 0}, "forceNum": 200, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "2": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "286a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "42b9", "guid": "27702", "offsetPos": {"x": 130, "y": 25, "z": 15}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c3fa", "guid": "51211", "offsetPos": {"x": 155, "y": 25, "z": 15}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4113", "guid": "27702", "offsetPos": {"x": 130, "y": 25, "z": 15}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9482", "guid": "151566", "offsetPos": {"x": 130, "y": 25, "z": 15}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e2f0", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 0.02, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "e993", "type": 1, "offsetLoc": {"x": 145, "y": 0, "z": 20}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 4, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 2, "dilationRate": 0, "dilationFrame": 0}], "4": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "eb88", "breakType": 2}], "5": [], "6": [], "8": [], "9": [], "10": []}</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>64</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>拳头普攻</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>怒气普攻3</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>17</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "58f2", "guid": "122529", "duration": 25, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1292", "guid": "160703", "offsetPos": {"x": 13, "y": -3, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "4d10", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "4": [], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e09f", "guid": "132631", "offsetPos": {"x": 100, "y": 0, "z": 20}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "#C136FF00", "colorHex1": ""}], "6": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "a0fc", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 6, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 6, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.7}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "67d2", "guid": "168948", "offsetPos": {"x": -10, "y": 0, "z": -108}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 2, "y": 1.3, "z": 1.3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ca1f", "guid": "13412", "offsetPos": {"x": 243, "y": 0, "z": 0}, "offsetRotation": {"x": -180, "y": -90, "z": -180}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "22f1", "guid": "27702", "offsetPos": {"x": 160, "y": 0, "z": 40}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3f19", "guid": "27702", "offsetPos": {"x": 160, "y": 0, "z": 40}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a1b8", "guid": "51209", "offsetPos": {"x": 175, "y": 0, "z": 40}, "offsetRotation": {"x": 90, "y": 0, "z": -90}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ca75", "guid": "151566", "offsetPos": {"x": 160, "y": 0, "z": 40}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "525d", "offsetPos": {"x": -100, "y": 0, "z": 0}, "forceNum": 700, "groundFriction": 0, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "1dfc", "type": 0, "offsetLoc": {"x": 350, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 6, "y": 4, "z": 4}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 3, "dilationRate": 0, "dilationFrame": 0}], "7": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cd2b", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 0.02, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "8": [], "9": [], "10": [], "11": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "dc63", "breakType": 2}], "12": [], "13": []}</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>65</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>单手剑普攻</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>怒气普攻1</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>9</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "764b", "guid": "117366", "duration": 11, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d766", "guid": "145503", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 17, "colorHex": "", "colorHex1": "Color|#004EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6303", "guid": "145503", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 18, "colorHex": "", "colorHex1": "Color|#004EFFFF"}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "9927", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "1": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "af27", "guid": "265136", "sound_volume": 1, "sound_innerRadius": 10000, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "2": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "8ef6", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "009f", "guid": "168950", "offsetPos": {"x": 150, "y": 10, "z": 30}, "offsetRotation": {"x": 30, "y": 3, "z": 180}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1706", "guid": "168950", "offsetPos": {"x": 150, "y": 10, "z": 30}, "offsetRotation": {"x": 30, "y": 3, "z": 180}, "offsetScale": {"x": 0.8, "y": 0.8, "z": 0.8}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1ecc", "guid": "168950", "offsetPos": {"x": 150, "y": 10, "z": 30}, "offsetRotation": {"x": 30, "y": 3, "z": 180}, "offsetScale": {"x": 1.2, "y": 1.2, "z": 1.2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "74e8", "guid": "151736", "offsetPos": {"x": 186, "y": -120, "z": -43}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e5b0", "guid": "151736", "offsetPos": {"x": 186, "y": 26, "z": 41}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "686a", "guid": "151736", "offsetPos": {"x": 186, "y": 185, "z": 144}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "f68a", "delayTime": 0, "bulletId": 31, "startLoc": {"x": 180, "y": 0, "z": 0}, "endType": 0, "endDis": 1000}], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "25ce", "guid": "151534", "offsetPos": {"x": 0, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "4": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "4c80", "breakType": 2}], "5": [], "6": [], "7": [], "8": []}</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>66</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>单手剑普攻</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>怒气普攻2</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>8</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "cc78", "guid": "117375", "duration": 10, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "205e", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4adb", "guid": "145503", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 17, "colorHex": "", "colorHex1": "Color|#004EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "515b", "guid": "145503", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 18, "colorHex": "", "colorHex1": "Color|#004EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9a30", "guid": "151534", "offsetPos": {"x": 0, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "f37b", "guid": "265136", "sound_volume": 1, "sound_innerRadius": 10000, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "1": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "87d5", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0166", "guid": "168950", "offsetPos": {"x": 100, "y": 10, "z": 35}, "offsetRotation": {"x": 150, "y": -3, "z": -180}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0d00", "guid": "168950", "offsetPos": {"x": 100, "y": 10, "z": 35}, "offsetRotation": {"x": 150, "y": -3, "z": -180}, "offsetScale": {"x": 1.2, "y": 1.2, "z": 1.2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a940", "guid": "168950", "offsetPos": {"x": 100, "y": 10, "z": 35}, "offsetRotation": {"x": 150, "y": -3, "z": -180}, "offsetScale": {"x": 0.8, "y": 0.8, "z": 0.8}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "11fa", "guid": "151736", "offsetPos": {"x": 200, "y": -120, "z": 110}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3436", "guid": "151736", "offsetPos": {"x": 200, "y": 26, "z": 43}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5853", "guid": "151736", "offsetPos": {"x": 200, "y": 185, "z": -53}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "4c8b", "delayTime": 0, "bulletId": 32, "startLoc": {"x": 100, "y": 0, "z": 0}, "endType": 0, "endDis": 1000}], "2": [], "3": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "6dd0", "breakType": 2}], "4": [], "5": [], "6": [], "7": []}</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>67</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>单手剑普攻</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>怒气普攻3</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>12</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "a44c", "guid": "117376", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "eb5d", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 1500, "groundFriction": 1, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "79b8", "guid": "145503", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -10, "slotIndex": 18, "colorHex": "", "colorHex1": "Color|#004EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f204", "guid": "145503", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -10, "slotIndex": 17, "colorHex": "", "colorHex1": "Color|#004EFFFF"}], "1": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7248", "guid": "151534", "offsetPos": {"x": 0, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "4": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "3306", "guid": "265136", "sound_volume": 1, "sound_innerRadius": 10000, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "5": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "7f62", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "918d", "guid": "168950", "offsetPos": {"x": 150, "y": 0, "z": 40}, "offsetRotation": {"x": -15, "y": 2, "z": 177}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d453", "guid": "168950", "offsetPos": {"x": 150, "y": 0, "z": 40}, "offsetRotation": {"x": -15, "y": 2, "z": 177}, "offsetScale": {"x": 1.2, "y": 1.2, "z": 1.2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2895", "guid": "168950", "offsetPos": {"x": 150, "y": 0, "z": 40}, "offsetRotation": {"x": -15, "y": 2, "z": 177}, "offsetScale": {"x": 0.8, "y": 0.8, "z": 0.8}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "97b2", "guid": "151736", "offsetPos": {"x": 150, "y": -176, "z": 71}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "50a5", "guid": "151736", "offsetPos": {"x": 150, "y": 0, "z": 38}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7abb", "guid": "151736", "offsetPos": {"x": 15, "y": 159, "z": -21}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "71b7", "delayTime": 0, "bulletId": 33, "startLoc": {"x": 100, "y": 0, "z": 0}, "endType": 0, "endDis": 1000}], "6": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "40d5", "guid": "265136", "sound_volume": 1, "sound_innerRadius": 10000, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "7": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "e783", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a7f9", "guid": "168950", "offsetPos": {"x": 150, "y": 0, "z": 40}, "offsetRotation": {"x": -150, "y": -3, "z": -180}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "06ad", "guid": "168950", "offsetPos": {"x": 150, "y": 0, "z": 40}, "offsetRotation": {"x": -150, "y": -3, "z": -180}, "offsetScale": {"x": 0.8, "y": 0.8, "z": 0.8}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0f8e", "guid": "168950", "offsetPos": {"x": 150, "y": 0, "z": 40}, "offsetRotation": {"x": -150, "y": -3, "z": -180}, "offsetScale": {"x": 1.2, "y": 1.2, "z": 1.2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#008EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3ae4", "guid": "151736", "offsetPos": {"x": 150, "y": 0, "z": 38}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2b60", "guid": "151736", "offsetPos": {"x": 150, "y": 164, "z": 130}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "56c2", "guid": "151736", "offsetPos": {"x": 150, "y": -156, "z": -56}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4450", "type": 0, "offsetLoc": {"x": 150, "y": 0, "z": 30}, "offsetRot": {"x": -30, "y": 0, "z": 0}, "LWH": {"x": 4, "y": 6, "z": 2}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 24, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "fe41", "delayTime": 0, "bulletId": 34, "startLoc": {"x": 100, "y": 0, "z": 0}, "endType": 0, "endDis": 1000}], "8": [], "9": [], "10": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "79ff", "breakType": 2}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>68</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>法杖普攻</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>怒气普攻1</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>7</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "62e7", "guid": "20258", "duration": 5, "animSlot": 1}], "2": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "1807", "delayTime": 0, "bulletId": 16, "startLoc": {"x": 135, "y": 55, "z": 50}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3556", "guid": "155715", "offsetPos": {"x": 145, "y": 55, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.8, "y": 0.8, "z": 0.8}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "af8c", "guid": "85156", "offsetPos": {"x": 145, "y": 55, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.7, "y": 0.7, "z": 0.7}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "baa2", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 0.05, "y": 2, "z": 2}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#DEC570FF"}], "3": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "cacb", "breakType": 2}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>69</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>法杖普攻</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>怒气普攻2</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>8</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "a79b", "guid": "156393", "duration": 10, "animSlot": 1}], "2": [], "3": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "7197", "delayTime": 0, "bulletId": 17, "startLoc": {"x": 130, "y": -55, "z": 74}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8289", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "289b", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6eee", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 0.05, "y": 3, "z": 3}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#DEC570FF"}], "4": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "94c5", "breakType": 2}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>70</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>双手剑普攻</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>怒气普攻1</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>14</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "d5a9", "guid": "217287", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "ec45", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "2": [], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "de44", "guid": "163340", "offsetPos": {"x": 100, "y": 0, "z": 20}, "offsetRotation": {"x": 17.44, "y": -25.57, "z": 53.96}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7100FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "aa76", "guid": "163340", "offsetPos": {"x": 100, "y": 0, "z": 20}, "offsetRotation": {"x": 17.44, "y": -25.57, "z": 53.96}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7100FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "426a", "guid": "163340", "offsetPos": {"x": 100, "y": 0, "z": 20}, "offsetRotation": {"x": 17.44, "y": -25.57, "z": 53.96}, "offsetScale": {"x": 2.5, "y": 2.5, "z": 2.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7100FF"}], "4": [], "5": [], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0dc3", "guid": "151562", "offsetPos": {"x": 342.36, "y": -18.03, "z": 34.5}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3500FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ca78", "guid": "151562", "offsetPos": {"x": 229.33, "y": -172.76, "z": 117.31}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3500FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5bc0", "guid": "151562", "offsetPos": {"x": 243.25, "y": 130.69, "z": -50.91}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3500FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "68c3", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "e511", "type": 0, "offsetLoc": {"x": 200, "y": -30, "z": 70}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 6, "z": 3}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 61, "dilationRate": 0, "dilationFrame": 0}], "7": [], "8": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "78b1", "breakType": 2}], "9": [], "10": [], "11": []}</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>71</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>双手剑普攻</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>怒气普攻2</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>20</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "f1fa", "guid": "217286", "duration": 25, "animSlot": 0}], "1": [], "2": [], "3": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "31c7", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "4": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6610", "guid": "163340", "offsetPos": {"x": 250, "y": 0, "z": 20}, "offsetRotation": {"x": 169.83, "y": -15.73, "z": -56.53}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7100FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4831", "guid": "163340", "offsetPos": {"x": 250, "y": 0, "z": 20}, "offsetRotation": {"x": 169.83, "y": -15.73, "z": -56.53}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7100FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0440", "guid": "163340", "offsetPos": {"x": 250, "y": 0, "z": 20}, "offsetRotation": {"x": 169.83, "y": -15.73, "z": -56.53}, "offsetScale": {"x": 2.5, "y": 2.5, "z": 2.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7100FF"}], "5": [], "6": [], "7": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "be83", "guid": "151562", "offsetPos": {"x": 214.2, "y": 272.93, "z": 101.52}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3500FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4943", "guid": "151562", "offsetPos": {"x": 158.34, "y": -220.41, "z": -64.61}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3500FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "353f", "guid": "151562", "offsetPos": {"x": 355.38, "y": 33.87, "z": 19.02}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3500FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "13e3", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "60df", "type": 0, "offsetLoc": {"x": 200, "y": -10, "z": 70}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5.5, "y": 7, "z": 3}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 62, "dilationRate": 0, "dilationFrame": 0}], "8": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "ef7d", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 1000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "9": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b1f5", "guid": "163340", "offsetPos": {"x": 100, "y": 0, "z": 20}, "offsetRotation": {"x": 3.33, "y": -5.3, "z": 57.78}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7100FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4689", "guid": "163340", "offsetPos": {"x": 100, "y": 0, "z": 20}, "offsetRotation": {"x": 3.33, "y": -5.3, "z": 57.78}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7100FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "97f7", "guid": "163340", "offsetPos": {"x": 100, "y": 0, "z": 20}, "offsetRotation": {"x": 3.33, "y": -5.3, "z": 57.78}, "offsetScale": {"x": 2.5, "y": 2.5, "z": 2.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7100FF"}], "10": [], "12": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8ce7", "guid": "151562", "offsetPos": {"x": 250.23, "y": -246.14, "z": 54.37}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3500FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c2ef", "guid": "151562", "offsetPos": {"x": 353.12, "y": 12.66, "z": 24.41}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3500FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f088", "guid": "151562", "offsetPos": {"x": 279.61, "y": 272.83, "z": -39.52}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3500FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "9890", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "7d9c", "type": 0, "offsetLoc": {"x": 230, "y": -10, "z": 70}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 6, "y": 8, "z": 3}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 63, "dilationRate": 0, "dilationFrame": 0}], "13": [], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "c826", "breakType": 2}], "15": [], "17": []}</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>72</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>大招技能组</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>拳头大招</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>24</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "b693", "guid": "121586", "duration": 15, "animSlot": 0}], "1": [], "2": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7382", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": 1, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "bd1f", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 90, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": 1, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8e0b", "guid": "168954", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -8, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#8896B8FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "6ad0", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "488a", "guid": "108248", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "3": [], "4": [], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "44d6", "guid": "160703", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -8, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "9": [], "10": [], "11": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "ad99", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.8}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a555", "guid": "135888", "offsetPos": {"x": 100, "y": 0, "z": -84}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "7644", "guid": "121586", "pauseCount": 5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "44c6", "guid": "27702", "offsetPos": {"x": 100, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 30, "y": 30, "z": 30}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1e93", "guid": "27702", "offsetPos": {"x": 100, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 100}, "offsetScale": {"x": 30, "y": 30, "z": 30}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4f0b", "guid": "51210", "offsetPos": {"x": 100, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 20, "y": 20, "z": 20}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "e78c", "type": 1, "offsetLoc": {"x": 100, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 46, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 12, "dilationRate": 0, "dilationFrame": 0}], "12": [], "13": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "013a", "breakType": 2}], "14": [], "15": [], "16": [], "17": [], "18": [], "20": [], "22": []}</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>73</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>大招技能组</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>单手剑大招</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>60</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "5382", "guid": "122524", "duration": 20, "animSlot": 0}], "2": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9662", "guid": "151568", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": 17, "colorHex": "", "colorHex1": "Color|#003FD2FF"}], "5": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "cc31", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4268", "guid": "151736", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -5, "slotIndex": 17, "colorHex": "", "colorHex1": "Color|0063D3FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fca3", "guid": "130743", "offsetPos": {"x": 1000, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "33b1", "guid": "20005", "offsetPos": {"x": 1000, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.8, "y": 2.8, "z": 2.8}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "d2f9", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 81, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Equip", "frameGuid": "8c06", "guid": "179425", "sourceType": 0, "equip_offsetPos": {"x": 1000, "y": 0, "z": 0}, "equip_offsetRotation": {"x": 0, "y": 0, "z": 0}, "equip_offsetScale": {"x": 1.66, "y": 1.66, "z": 1.66}, "equip_socket": 23}, {"frameNodeType": "MotionFrameNode_Equip", "frameGuid": "917b", "guid": "47521", "sourceType": 0, "equip_offsetPos": {"x": 1000, "y": 0, "z": 0}, "equip_offsetRotation": {"x": 0, "y": 0, "z": 0}, "equip_offsetScale": {"x": 1.21, "y": 1.21, "z": 1.21}, "equip_socket": 23}], "7": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "7edb", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 82, "dilationRate": 0, "dilationFrame": 0}], "11": [{"frameNodeType": "MotionFrameNode_Camera", "frameGuid": "af4a", "camrea_offsetPos": {"x": -260.9088439941406, "y": 129.50955200195312, "z": 105.499755859375}, "camrea_offsetRotation": {"x": 0.9863521456718445, "y": -0.14275288581848145, "z": -0.08204572647809982}, "camrea_during": 0.1, "camrea_keepFrame": 25, "resetTime": 0.1}], "12": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "e434", "guid": "111103", "duration": 7, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "70bd", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "10af", "guid": "168950", "offsetPos": {"x": 595, "y": 0, "z": 200}, "offsetRotation": {"x": -20, "y": 0, "z": 180}, "offsetScale": {"x": 3.85, "y": 3.85, "z": 3.85}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "680b", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 83, "dilationRate": 0, "dilationFrame": 0}], "13": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5276", "guid": "137227", "offsetPos": {"x": 885, "y": 0, "z": 350}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "14": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "73c8", "guid": "168950", "offsetPos": {"x": 885, "y": 0, "z": 200}, "offsetRotation": {"x": -160, "y": 0, "z": -180}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "96d1", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 84, "dilationRate": 0, "dilationFrame": 0}], "15": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fd27", "guid": "137227", "offsetPos": {"x": 885, "y": 0, "z": 350}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "16": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "b9d1", "guid": "111102", "duration": 7, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "2d7e", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e612", "guid": "168950", "offsetPos": {"x": 885, "y": 0, "z": 200}, "offsetRotation": {"x": -160, "y": 0, "z": -180}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "6e41", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 85, "dilationRate": 0, "dilationFrame": 0}], "17": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6384", "guid": "137227", "offsetPos": {"x": 885, "y": 0, "z": 350}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "18": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "67e1", "guid": "168950", "offsetPos": {"x": 595, "y": 0, "z": 200}, "offsetRotation": {"x": 140, "y": 0, "z": -180}, "offsetScale": {"x": 3.85, "y": 3.85, "z": 3.85}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "44a0", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 83, "dilationRate": 0, "dilationFrame": 0}], "19": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "992f", "guid": "137227", "offsetPos": {"x": 885, "y": 0, "z": 350}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "20": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "9f2a", "guid": "111101", "duration": 7, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "a2fa", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ffe4", "guid": "168950", "offsetPos": {"x": 595, "y": 0, "z": 200}, "offsetRotation": {"x": 140, "y": 0, "z": -180}, "offsetScale": {"x": 3.85, "y": 3.85, "z": 3.85}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2171", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 84, "dilationRate": 0, "dilationFrame": 0}], "21": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "70c1", "guid": "137227", "offsetPos": {"x": 885, "y": 0, "z": 350}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "23": [], "24": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "1311", "guid": "29744", "duration": 14, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "4e57", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0070", "guid": "168950", "offsetPos": {"x": 885, "y": 0, "z": 200}, "offsetRotation": {"x": -160, "y": 0, "z": -180}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "ddba", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 85, "dilationRate": 0, "dilationFrame": 0}], "25": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e6aa", "guid": "137227", "offsetPos": {"x": 885, "y": 0, "z": 350}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "26": [], "27": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "63c2", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f047", "guid": "168950", "offsetPos": {"x": 885, "y": 0, "z": 200}, "offsetRotation": {"x": -160, "y": 0, "z": -180}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "5273", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 83, "dilationRate": 0, "dilationFrame": 0}], "28": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d4ac", "guid": "168950", "offsetPos": {"x": 595, "y": 0, "z": 200}, "offsetRotation": {"x": -20, "y": 0, "z": 180}, "offsetScale": {"x": 3.85, "y": 3.85, "z": 3.85}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e7d2", "guid": "137227", "offsetPos": {"x": 885, "y": 0, "z": 350}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "0fc4", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 84, "dilationRate": 0, "dilationFrame": 0}], "30": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "9e21", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "115c", "guid": "168950", "offsetPos": {"x": 595, "y": 0, "z": 200}, "offsetRotation": {"x": -20, "y": 0, "z": 180}, "offsetScale": {"x": 3.85, "y": 3.85, "z": 3.85}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "cbfb", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 85, "dilationRate": 0, "dilationFrame": 0}], "31": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "063e", "guid": "168950", "offsetPos": {"x": 885, "y": 0, "z": 200}, "offsetRotation": {"x": -50, "y": 0, "z": 180}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "31dd", "guid": "137227", "offsetPos": {"x": 885, "y": 0, "z": 350}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "213c", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 83, "dilationRate": 0, "dilationFrame": 0}], "33": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "479a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a24f", "guid": "168950", "offsetPos": {"x": 885, "y": 0, "z": 200}, "offsetRotation": {"x": -50, "y": 0, "z": 180}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2974", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 84, "dilationRate": 0, "dilationFrame": 0}], "34": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "055c", "guid": "137227", "offsetPos": {"x": 885, "y": 0, "z": 350}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "3ecb", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 85, "dilationRate": 0, "dilationFrame": 0}], "35": [], "36": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "c356", "guid": "85121", "duration": 30, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Camera", "frameGuid": "f464", "camrea_offsetPos": {"x": 55.61063003540039, "y": -56.70420837402344, "z": 220.6416015625}, "camrea_offsetRotation": {"x": -0.7662395, "y": 0.6229296922683716, "z": -0.15759439766407013}, "camrea_during": 0.5, "camrea_keepFrame": 11, "resetTime": 0.1}], "39": [], "40": [], "41": [], "42": [], "43": [], "44": [], "45": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2b0d", "guid": "151568", "offsetPos": {"x": 2, "y": 14, "z": 1}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.7, "y": 0.7, "z": 0.7}, "count": -10, "slotIndex": 5, "colorHex": "", "colorHex1": "Color|#0073D2FF"}], "46": [], "47": [], "48": [], "49": [], "50": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "6d96", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 20, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 20, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.7}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8bd6", "guid": "150927", "offsetPos": {"x": 1000, "y": 0, "z": 255}, "offsetRotation": {"x": 0, "y": 0, "z": 90}, "offsetScale": {"x": 40, "y": 16, "z": 16}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0075FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5a9e", "guid": "150927", "offsetPos": {"x": 1000, "y": 0, "z": 255}, "offsetRotation": {"x": 0, "y": 10, "z": 150}, "offsetScale": {"x": 40, "y": 16, "z": 16}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0075FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4437", "guid": "150927", "offsetPos": {"x": 1000, "y": 0, "z": 255}, "offsetRotation": {"x": 27.11, "y": -32.8, "z": -135}, "offsetScale": {"x": 40, "y": 16, "z": 16}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0075FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3b3d", "guid": "150927", "offsetPos": {"x": 1000, "y": 0, "z": 255}, "offsetRotation": {"x": 0, "y": 10, "z": 0}, "offsetScale": {"x": 40, "y": 16, "z": 16}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0075FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "eb9f", "guid": "150927", "offsetPos": {"x": 1000, "y": 0, "z": 255}, "offsetRotation": {"x": 0, "y": 10, "z": 60}, "offsetScale": {"x": 40, "y": 16, "z": 16}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0075FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d32d", "guid": "150927", "offsetPos": {"x": 1000, "y": 0, "z": 255}, "offsetRotation": {"x": 27.11, "y": -32, "z": 134}, "offsetScale": {"x": 40, "y": 16, "z": 16}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0075FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "49b0", "guid": "151556", "offsetPos": {"x": 1000, "y": 0, "z": 255}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 25, "y": 25, "z": 25}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0075FFFF"}], "51": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "d8f1", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 22.6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 86, "dilationRate": 0, "dilationFrame": 0}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>74</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>大招技能组</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>法杖大招</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>31</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "b4df", "guid": "156436", "duration": 20, "animSlot": 1}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "d0fe", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 48, "dilationRate": 0, "dilationFrame": 0}], "6": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "35b6", "guid": "156436", "pauseCount": 15}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d047", "guid": "168954", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 3}, "count": -20, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFDB00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1658", "guid": "160701", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.3, "y": 1.3, "z": 3}, "count": -20, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFB200FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3575", "guid": "146785", "offsetPos": {"x": 190, "y": 0, "z": 120}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -20, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFC700FF"}], "7": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cebb", "guid": "160748", "offsetPos": {"x": 270, "y": 0, "z": 120}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 8, "y": 8, "z": 8}, "count": -20, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFB700FF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "7b5c", "type": 0, "offsetLoc": {"x": 3600, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 70, "y": 7.5, "z": 7.5}, "range": 1, "checkCount": 10, "checkInterval": 0.2, "keepFrameCount": 20, "rectSocket": 0, "effectid": 51, "dilationRate": 0, "dilationFrame": 0, "cameraShakeId": 0, "isShake": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "8353", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 8, "xFrequency": 6, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 8, "zFrequency": 6, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 2}], "8": [], "9": [], "10": [], "27": [], "28": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "158c", "breakType": 1}]}</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>75</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>大招技能组</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>双手剑大招</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>17</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "90e4", "guid": "119910", "duration": 30, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c6e2", "guid": "156437", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.75, "y": 0.75, "z": 0.75}, "count": -10, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FF2B00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5c67", "guid": "156437", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.75, "y": 0.75, "z": 0.75}, "count": -10, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FF2B00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b7f1", "guid": "162217", "offsetPos": {"x": 4.61, "y": 2.26, "z": 0.72}, "offsetRotation": {"x": -5.33, "y": -14.76, "z": 0.91}, "offsetScale": {"x": 3, "y": 3, "z": 2.1}, "count": -10, "slotIndex": 16, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4c78", "guid": "162431", "offsetPos": {"x": 30, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 1}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FF4300FF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "d5ba", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "7": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "e188", "delayTime": 0, "bulletId": 30, "startLoc": {"x": 350, "y": -50, "z": 0}, "endType": 0, "endDis": 6000}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "7cf7", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 8, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 8, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.4}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6281", "guid": "131516", "offsetPos": {"x": 200, "y": -50, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -4, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7E00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1fa8", "guid": "29393", "offsetPos": {"x": 200, "y": -50, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -4, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF7E00FF"}], "9": [], "10": [], "11": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "43bc", "breakType": 2}], "12": []}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：update skill punch animation
</commit_message>
<xml_diff>
--- a/battleworld/Excel/MotionClip_技能数据.xlsx
+++ b/battleworld/Excel/MotionClip_技能数据.xlsx
@@ -649,7 +649,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "211a", "guid": "122528", "duration": 12, "animSlot": 0}], "2": [], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d3fc", "guid": "92838", "offsetPos": {"x": 450, "y": 0, "z": 30}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Move", "frameGuid": "6b5f", "move_offsetPos": {"x": 200, "y": 0, "z": 0}, "move_isFlash": 0, "move_count": 0}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "93cb", "guid": "209223", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "4": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "845a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1aab", "guid": "151566", "offsetPos": {"x": 100, "y": 0, "z": 10}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "ea41", "type": 0, "offsetLoc": {"x": 155, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 2.5, "y": 2.5, "z": 2.5}, "range": 3, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 1, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "02a5", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 0.05, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "5": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "3bfa", "breakType": 2}], "6": [], "7": [], "8": [], "9": [], "10": [], "12": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "211a", "guid": "122528", "duration": 12, "animSlot": 0}], "2": [], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d3fc", "guid": "92838", "offsetPos": {"x": 450, "y": 0, "z": 30}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Move", "frameGuid": "6b5f", "move_offsetPos": {"x": 200, "y": 0, "z": 0}, "move_isFlash": 0, "move_count": 0}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "93cb", "guid": "209223", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "4": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "845a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1aab", "guid": "151566", "offsetPos": {"x": 100, "y": 0, "z": 10}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "ea41", "type": 0, "offsetLoc": {"x": 155, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 2.5, "y": 2.5, "z": 2.5}, "range": 3, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 1, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "02a5", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 0.05, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "5": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "3bfa", "breakType": 1}], "6": [], "7": [], "8": [], "9": [], "10": [], "12": []}</t>
         </is>
       </c>
     </row>
@@ -672,7 +672,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "58f2", "guid": "121600", "duration": 15, "animSlot": 0}], "1": [], "2": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "286a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 20, "xFrequency": 2, "xWaveform": 1, "yAmplitude": 20, "yFrequency": 2, "yWaveform": 1, "zAmplitude": 20, "zFrequency": 2, "zWaveform": 1, "fovAmplitude": 5, "fovFrequency": 4, "fovWaveform": 1, "keepTime": 0.05}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9482", "guid": "92821", "offsetPos": {"x": 0, "y": 0, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7ddb", "guid": "151568", "offsetPos": {"x": 250, "y": 0, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "8b73", "guid": "209223", "sound_volume": 100, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "3": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "e993", "type": 1, "offsetLoc": {"x": 145, "y": 0, "z": 20}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 2.3, "y": 2.3, "z": 2.3}, "range": 4, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 2, "dilationRate": 0, "dilationFrame": 0}], "4": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "eb88", "breakType": 2}], "5": [], "6": [], "8": [], "9": [], "10": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "58f2", "guid": "121600", "duration": 15, "animSlot": 0}], "1": [], "2": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "286a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 20, "xFrequency": 2, "xWaveform": 1, "yAmplitude": 20, "yFrequency": 2, "yWaveform": 1, "zAmplitude": 20, "zFrequency": 2, "zWaveform": 1, "fovAmplitude": 5, "fovFrequency": 4, "fovWaveform": 1, "keepTime": 0.05}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9482", "guid": "92821", "offsetPos": {"x": 0, "y": 0, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "8b73", "guid": "209223", "sound_volume": 100, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "3": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "e993", "type": 0, "offsetLoc": {"x": 175, "y": 0, "z": 20}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 3, "y": 5, "z": 3}, "range": 4, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 2, "dilationRate": 0, "dilationFrame": 0}], "4": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "eb88", "breakType": 2}], "5": [], "6": [], "8": [], "9": [], "10": []}</t>
         </is>
       </c>
     </row>
@@ -695,7 +695,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "58f2", "guid": "269289", "duration": 25, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1292", "guid": "160703", "offsetPos": {"x": 13, "y": -3, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "4d10", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2500, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "4": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "5377", "guid": "205238", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e09f", "guid": "132631", "offsetPos": {"x": 100, "y": 0, "z": 20}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "#C136FF00", "colorHex1": ""}], "6": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "a0fc", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 6, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 6, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.7}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "67d2", "guid": "168948", "offsetPos": {"x": -10, "y": 0, "z": -108}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 2, "y": 1.3, "z": 1.3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ca1f", "guid": "13412", "offsetPos": {"x": 243, "y": 0, "z": 0}, "offsetRotation": {"x": -180, "y": -90, "z": -180}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3f19", "guid": "27702", "offsetPos": {"x": 160, "y": 0, "z": 40}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ca75", "guid": "151566", "offsetPos": {"x": 160, "y": 0, "z": 40}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "525d", "offsetPos": {"x": -100, "y": 0, "z": 0}, "forceNum": 700, "groundFriction": 0, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "1dfc", "type": 0, "offsetLoc": {"x": 350, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 6, "y": 4, "z": 4}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 3, "dilationRate": 0, "dilationFrame": 0}], "7": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cd2b", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 0.02, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "8": [], "9": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "cb27", "breakType": 2}], "10": [], "11": [], "12": [], "13": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "58f2", "guid": "269289", "duration": 21, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1292", "guid": "160703", "offsetPos": {"x": 13, "y": -3, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "4d10", "offsetPos": {"x": 300, "y": 0, "z": 10}, "forceNum": 2500, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "3": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "2236", "guid": "205238", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "4": [], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e09f", "guid": "132631", "offsetPos": {"x": 100, "y": 0, "z": 20}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "#C136FF00", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "ac4c", "offsetPos": {"x": -100, "y": 0, "z": 0}, "forceNum": 1400, "groundFriction": 1, "gravityScale": 1, "gravityTime": 0}], "6": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "a0fc", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 5, "xFrequency": 6, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 6, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.7}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "67d2", "guid": "168948", "offsetPos": {"x": -10, "y": 0, "z": -108}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 2, "y": 1.3, "z": 1.3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ca1f", "guid": "13412", "offsetPos": {"x": 243, "y": 0, "z": 0}, "offsetRotation": {"x": -180, "y": -90, "z": -180}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3f19", "guid": "27702", "offsetPos": {"x": 160, "y": 0, "z": 40}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ca75", "guid": "151566", "offsetPos": {"x": 160, "y": 0, "z": 40}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "1dfc", "type": 0, "offsetLoc": {"x": 350, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 6, "y": 4, "z": 4}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 3, "dilationRate": 0, "dilationFrame": 0}], "7": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cd2b", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 0.02, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "8": [], "9": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "cb27", "breakType": 2}], "10": [], "11": [], "12": [], "13": []}</t>
         </is>
       </c>
     </row>
@@ -902,7 +902,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "50b8", "guid": "121609", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4500", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "4": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "1aeb", "guid": "205238", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d08f", "guid": "200918", "offsetPos": {"x": 80, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.4, "y": 1.4, "z": 1.4}, "count": -15, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF6C00"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e6f9", "guid": "14329", "offsetPos": {"x": 400, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "25ed", "guid": "14329", "offsetPos": {"x": -400, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "74b3", "guid": "14329", "offsetPos": {"x": 0, "y": 400, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e068", "guid": "14329", "offsetPos": {"x": 0, "y": -400, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "c8c3", "type": 0, "offsetLoc": {"x": 400, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 5, "z": 8}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 5, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "1add", "type": 0, "offsetLoc": {"x": -400, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 5, "z": 8}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 5, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8aaa", "guid": "14329", "offsetPos": {"x": 0, "y": 400, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c647", "guid": "14329", "offsetPos": {"x": 0, "y": 400, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "e53c", "type": 0, "offsetLoc": {"x": 0, "y": 400, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 5, "z": 8}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 5, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "3a89", "type": 0, "offsetLoc": {"x": 0, "y": -400, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 5, "z": 8}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 5, "dilationRate": 0, "dilationFrame": 0}], "6": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "d18c", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "7": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "81a3", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "8": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "4f4f", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "9": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "5118", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "10": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "16bf", "breakType": 2}], "16": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "50b8", "guid": "121609", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4500", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "4": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "1aeb", "guid": "205238", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d08f", "guid": "200918", "offsetPos": {"x": 80, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.4, "y": 1.4, "z": 1.4}, "count": -15, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF6C00"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e6f9", "guid": "14329", "offsetPos": {"x": 400, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "25ed", "guid": "14329", "offsetPos": {"x": -400, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "74b3", "guid": "14329", "offsetPos": {"x": 0, "y": 400, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e068", "guid": "14329", "offsetPos": {"x": 0, "y": -400, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "c8c3", "type": 0, "offsetLoc": {"x": 400, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 5, "z": 8}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 5, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "1add", "type": 0, "offsetLoc": {"x": -400, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 5, "z": 8}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 5, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8aaa", "guid": "14329", "offsetPos": {"x": 0, "y": 400, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c647", "guid": "14329", "offsetPos": {"x": 0, "y": 400, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.4, "y": 0.4, "z": 0.4}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "e53c", "type": 0, "offsetLoc": {"x": 0, "y": 400, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 5, "z": 8}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 5, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "3a89", "type": 0, "offsetLoc": {"x": 0, "y": -400, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 5, "z": 8}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 5, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "140e", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 5, "z": 8}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 5, "dilationRate": 0, "dilationFrame": 0}], "6": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "d18c", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "7": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "81a3", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "8": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "4f4f", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "9": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "5118", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 5, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "10": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "16bf", "breakType": 2}], "16": []}</t>
         </is>
       </c>
     </row>
@@ -925,7 +925,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "3ec3", "guid": "8350", "duration": 15, "animSlot": 0}], "1": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f80b", "guid": "132860", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": 16, "colorHex": "#AE00FF00", "colorHex1": ""}], "4": [], "9": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "2af4", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "396b", "guid": "57200", "offsetPos": {"x": 400, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "08cf", "guid": "51209", "offsetPos": {"x": 400, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4e3d", "guid": "27702", "offsetPos": {"x": 400, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8b60", "guid": "151534", "offsetPos": {"x": 400, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 12, "y": 12, "z": 12}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2776", "type": 1, "offsetLoc": {"x": 400, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 9, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 6, "dilationRate": 0, "dilationFrame": 0}], "11": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "3eac", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 6, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 6, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "649a", "guid": "57200", "offsetPos": {"x": 1000, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "823e", "guid": "51209", "offsetPos": {"x": 1000, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5fde", "guid": "27702", "offsetPos": {"x": 1000, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 9, "y": 9, "z": 9}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c689", "guid": "151534", "offsetPos": {"x": 1000, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 18, "y": 18, "z": 18}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9253", "guid": "151534", "offsetPos": {"x": 1000, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 18, "y": 18, "z": 18}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "3a8e", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 13.5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 7, "dilationRate": 0, "dilationFrame": 0}], "12": [], "13": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "88ad", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 8, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 8, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6183", "guid": "57200", "offsetPos": {"x": 2000, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3484", "guid": "51209", "offsetPos": {"x": 2000, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 8, "y": 8, "z": 8}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b57c", "guid": "27702", "offsetPos": {"x": 2000, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 12, "y": 12, "z": 12}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a543", "guid": "151534", "offsetPos": {"x": 2000, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 24, "y": 24, "z": 24}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "b087", "type": 1, "offsetLoc": {"x": 2000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 18, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 8, "dilationRate": 0, "dilationFrame": 0}], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "8152", "breakType": 2}], "15": [], "16": [], "17": [], "19": [], "20": [], "21": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "3ec3", "guid": "117324", "duration": 18, "animSlot": 0}], "1": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f80b", "guid": "132860", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": 16, "colorHex": "#AE00FF00", "colorHex1": ""}], "4": [], "7": [{"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "7e5c", "guid": "205238", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "8": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "950e", "guid": "89080", "offsetPos": {"x": 450, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "Color|#FFFFFFFF", "colorHex1": ""}], "9": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "2af4", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2776", "type": 1, "offsetLoc": {"x": 400, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 9, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 6, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "8e59", "guid": "205238", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "10": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cf20", "guid": "89080", "offsetPos": {"x": 1050, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3.2, "y": 3.2, "z": 3.2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "11": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "3eac", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 6, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 6, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "3a8e", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 13.5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 7, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "0596", "guid": "205238", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "12": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "292e", "guid": "89080", "offsetPos": {"x": 2050, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3.5, "y": 3.5, "z": 3.5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "13": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "88ad", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 8, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 8, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "b087", "type": 1, "offsetLoc": {"x": 2000, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 18, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 8, "dilationRate": 0, "dilationFrame": 0}], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "8152", "breakType": 2}], "15": [], "16": [], "17": [], "19": [], "20": [], "21": []}</t>
         </is>
       </c>
     </row>
@@ -944,11 +944,11 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "6c78", "guid": "29732", "duration": 16, "animSlot": 0}], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "50c0", "guid": "27702", "offsetPos": {"x": 200, "y": 180, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b94e", "guid": "27702", "offsetPos": {"x": 200, "y": -180, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "06ee", "guid": "14328", "offsetPos": {"x": 200, "y": 180, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -7, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8d7b", "guid": "14328", "offsetPos": {"x": 200, "y": -180, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -7, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6662", "guid": "51209", "offsetPos": {"x": 200, "y": 180, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -7, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "aa68", "guid": "51209", "offsetPos": {"x": 200, "y": -180, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -7, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "eb37", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "f906", "type": 1, "offsetLoc": {"x": 200, "y": 180, "z": -50}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 4, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 9, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "602d", "type": 1, "offsetLoc": {"x": 200, "y": -180, "z": -50}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 4, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 9, "dilationRate": 0, "dilationFrame": 0}], "4": [], "11": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d72f", "guid": "27702", "offsetPos": {"x": 180, "y": 0, "z": 50}, "offsetRotation": {"x": 90, "y": 0, "z": 90}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0447", "guid": "27702", "offsetPos": {"x": 180, "y": 0, "z": 50}, "offsetRotation": {"x": 90, "y": 0, "z": -90}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f8fa", "guid": "51209", "offsetPos": {"x": 180, "y": 0, "z": 70}, "offsetRotation": {"x": 90, "y": 0, "z": -90}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1f46", "guid": "218416", "offsetPos": {"x": 250, "y": 0, "z": 70}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 5, "y": 2, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "25cf", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 15, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 15, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "8897", "type": 0, "offsetLoc": {"x": 1565, "y": 0, "z": 70}, "offsetRot": {"x": 0, "y": 0, "z": -90}, "LWH": {"x": 5, "y": 31, "z": 5}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 10, "dilationRate": 0, "dilationFrame": 0}], "13": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "1e37", "breakType": 2}], "14": [], "18": [], "19": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "6c78", "guid": "121599", "duration": 24, "animSlot": 0}], "1": [], "2": [{"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "9a55", "guid": "137565", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "3": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "eb37", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "602d", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 0, "y": 1, "z": 1}, "range": 4, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 9, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1282", "guid": "135889", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#1252C3"}], "4": [], "5": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "63cb", "guid": "122522", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "591c", "guid": "160703", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#1252C3"}], "7": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "218b", "guid": "122522", "pauseCount": 1}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "829b", "guid": "199437", "sound_volume": 5, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "8": [], "9": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fa9e", "guid": "135894", "offsetPos": {"x": 200, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#1252C3"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "011b", "type": 0, "offsetLoc": {"x": 1050, "y": 0, "z": 70}, "offsetRot": {"x": 0, "y": 0, "z": 90}, "LWH": {"x": 5, "y": 20, "z": 5}, "range": 4, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 10, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "4551", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 15, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 15, "yFrequency": 4, "yWaveform": 1, "zAmplitude": 0, "zFrequency": 0, "zWaveform": 0, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}], "11": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "1df8", "breakType": 2}], "13": [], "14": []}</t>
         </is>
       </c>
     </row>
@@ -967,11 +967,11 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "0b4a", "guid": "108415", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "2592", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fe68", "guid": "162432", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "9c60", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 47, "dilationRate": 0, "dilationFrame": 0}], "2": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d216", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -7, "slotIndex": 16, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f123", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -7, "slotIndex": 16, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "78f2", "guid": "168954", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -8, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4d0f", "guid": "160703", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -8, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "4": [], "5": [], "7": [], "10": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "886c", "guid": "108414", "duration": 22, "animSlot": 0}], "13": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "47da", "guid": "27702", "offsetPos": {"x": 180, "y": 15, "z": 50}, "offsetRotation": {"x": 90, "y": 0, "z": 90}, "offsetScale": {"x": 7, "y": 7, "z": 7}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8bf1", "guid": "27702", "offsetPos": {"x": 180, "y": 15, "z": 50}, "offsetRotation": {"x": 90, "y": 0, "z": -90}, "offsetScale": {"x": 7, "y": 7, "z": 7}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8c03", "guid": "51209", "offsetPos": {"x": 180, "y": 0, "z": 70}, "offsetRotation": {"x": 90, "y": 0, "z": -90}, "offsetScale": {"x": 8, "y": 8, "z": 8}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "1b14", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8362", "guid": "89089", "offsetPos": {"x": 150, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "78c5", "guid": "89089", "offsetPos": {"x": 150, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "eaad", "guid": "123626", "offsetPos": {"x": 150, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -12, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "b56c", "type": 1, "offsetLoc": {"x": 200, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 15, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 11, "dilationRate": 0, "dilationFrame": 0}], "14": [], "15": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "8f93", "breakType": 2}], "19": [], "22": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "0b4a", "guid": "285550", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "2592", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fe68", "guid": "162432", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "9c60", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 47, "dilationRate": 0, "dilationFrame": 0}], "2": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d216", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": 16, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f123", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": 16, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "78f2", "guid": "168954", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -6, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4d0f", "guid": "160703", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -6, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "4": [], "5": [], "6": [], "7": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "01d5", "guid": "269275", "duration": 22, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "25e8", "guid": "201180", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "8": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "d205", "guid": "269275", "pauseCount": 2}], "10": [], "11": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "c728", "guid": "117409", "duration": 20, "animSlot": 0}], "12": [], "13": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "1b14", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "eaad", "guid": "123626", "offsetPos": {"x": 150, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -15, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "b56c", "type": 1, "offsetLoc": {"x": 200, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 15, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 11, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "adae", "offsetPos": {"x": -200, "y": 0, "z": 0}, "forceNum": 3000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1ef3", "guid": "295657", "offsetPos": {"x": 800, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.5, "y": 2.5, "z": 2.5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFBF8FF"}], "14": [], "15": [], "16": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "f742", "breakType": 1}], "17": [], "19": []}</t>
         </is>
       </c>
     </row>
@@ -990,11 +990,11 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "b693", "guid": "121586", "duration": 15, "animSlot": 0}], "1": [], "2": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7382", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": 1, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "bd1f", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 90, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": 1, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8e0b", "guid": "168954", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -8, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#8896B8FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "6ad0", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "488a", "guid": "108248", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "3": [], "4": [], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "44d6", "guid": "160703", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -8, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "9": [], "10": [], "11": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "ad99", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.8}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a555", "guid": "135888", "offsetPos": {"x": 100, "y": 0, "z": -84}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "7644", "guid": "121586", "pauseCount": 5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "44c6", "guid": "27702", "offsetPos": {"x": 100, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 15, "y": 15, "z": 15}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1e93", "guid": "27702", "offsetPos": {"x": 100, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 100}, "offsetScale": {"x": 15, "y": 15, "z": 15}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4f0b", "guid": "51210", "offsetPos": {"x": 100, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "e78c", "type": 1, "offsetLoc": {"x": 100, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 23, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 12, "dilationRate": 0, "dilationFrame": 0}], "12": [], "13": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "013a", "breakType": 2}], "14": [], "15": [], "16": [], "17": [], "18": [], "20": [], "22": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "b693", "guid": "285732", "duration": 25, "animSlot": 0}], "1": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "63ad", "offsetPos": {"x": 0, "y": 0, "z": 100}, "forceNum": 1500, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "2": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7382", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -6, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "bd1f", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 90, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -6, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8e0b", "guid": "168954", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -8, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#8896B8FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "6ad0", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "488a", "guid": "108248", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -6, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "3": [], "4": [], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "44d6", "guid": "160703", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -8, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "6": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "3b7a", "offsetPos": {"x": 0, "y": 0, "z": 100}, "forceNum": -10000, "groundFriction": 2, "gravityScale": 6, "gravityTime": 1}], "7": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "4698", "guid": "205645", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "8": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "be10", "guid": "135888", "offsetPos": {"x": 100, "y": 0, "z": -200}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ee34", "guid": "27702", "offsetPos": {"x": 100, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 15, "y": 15, "z": 15}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "fe7c", "type": 1, "offsetLoc": {"x": 100, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 23, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 12, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "a2c0", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.8}], "9": [], "10": [], "11": [], "12": [], "13": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "013a", "breakType": 2}], "14": [], "15": [], "16": [], "17": [], "18": [], "20": []}</t>
         </is>
       </c>
     </row>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "3eb1", "guid": "85030", "duration": 30, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cda9", "guid": "160703", "offsetPos": {"x": 13, "y": -3, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -13, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "3": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "29d3", "offsetPos": {"x": 200, "y": 0, "z": 250}, "forceNum": 1700, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "5": [], "6": [], "12": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "dd49", "guid": "101408", "offsetPos": {"x": 200, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "07a6", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d4f3", "guid": "51209", "offsetPos": {"x": 200, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 8, "y": 8, "z": 8}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9f9a", "guid": "27702", "offsetPos": {"x": 200, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8305", "guid": "168949", "offsetPos": {"x": 200, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "72c3", "guid": "51210", "offsetPos": {"x": 200, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "13": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2660", "guid": "130743", "offsetPos": {"x": 200, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "d7e1", "type": 1, "offsetLoc": {"x": 150, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 12, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 15, "dilationRate": 0, "dilationFrame": 0}], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "c2c9", "breakType": 2}], "15": [], "17": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "3eb1", "guid": "85030", "duration": 30, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cda9", "guid": "160703", "offsetPos": {"x": 13, "y": -3, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -13, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "3": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "29d3", "offsetPos": {"x": 200, "y": 0, "z": 250}, "forceNum": 1700, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "5": [], "6": [], "8": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "398b", "guid": "199420", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "9": [], "11": [], "12": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "dd49", "guid": "101408", "offsetPos": {"x": 200, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "07a6", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9f9a", "guid": "27702", "offsetPos": {"x": 200, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8305", "guid": "168949", "offsetPos": {"x": 200, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "13": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2660", "guid": "130743", "offsetPos": {"x": 200, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "d7e1", "type": 1, "offsetLoc": {"x": 150, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 12, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 15, "dilationRate": 0, "dilationFrame": 0}], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "c2c9", "breakType": 2}], "15": [], "17": []}</t>
         </is>
       </c>
     </row>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "de34", "guid": "117541", "duration": 23, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0e06", "guid": "153611", "offsetPos": {"x": 0, "y": 0, "z": -85}, "offsetRotation": {"x": -180, "y": 0, "z": -180}, "offsetScale": {"x": 3, "y": 3, "z": 0.05}, "count": -2, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7830", "guid": "153611", "offsetPos": {"x": 0, "y": 0, "z": -85}, "offsetRotation": {"x": -180, "y": 0, "z": -180}, "offsetScale": {"x": 2, "y": 2, "z": 0.05}, "count": -2, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d4bf", "guid": "108249", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -4, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c183", "guid": "108247", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -4, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "6857", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "007b", "guid": "88441", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "5": [], "6": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "6e33", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 8, "xFrequency": 6, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 8, "zFrequency": 6, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6431", "guid": "27702", "offsetPos": {"x": 138, "y": 10, "z": 25}, "offsetRotation": {"x": 0, "y": 70, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "720d", "guid": "27702", "offsetPos": {"x": 138, "y": 10, "z": 25}, "offsetRotation": {"x": 0, "y": -70, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "22f7", "guid": "51209", "offsetPos": {"x": 128, "y": 10, "z": 25}, "offsetRotation": {"x": -180, "y": -70, "z": 180}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3e7f", "guid": "130643", "offsetPos": {"x": 94, "y": 0, "z": 20}, "offsetRotation": {"x": -45, "y": 0, "z": -90}, "offsetScale": {"x": 3, "y": 3, "z": 1.5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2010", "type": 1, "offsetLoc": {"x": 180, "y": 10, "z": 25}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 16, "dilationRate": 0, "dilationFrame": 0}], "7": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2d28", "guid": "27702", "offsetPos": {"x": 182, "y": 10, "z": 140}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "32c6", "guid": "27702", "offsetPos": {"x": 182, "y": 10, "z": 140}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "148b", "guid": "51209", "offsetPos": {"x": 182, "y": 10, "z": 140}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "e6d8", "type": 1, "offsetLoc": {"x": 183, "y": 10, "z": 140}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 17, "dilationRate": 0, "dilationFrame": 0}], "8": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8ac9", "guid": "27702", "offsetPos": {"x": 133, "y": 10, "z": 236}, "offsetRotation": {"x": -180, "y": 60, "z": 180}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "66b3", "guid": "27702", "offsetPos": {"x": 133, "y": 10, "z": 236}, "offsetRotation": {"x": 0, "y": -60, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "bcbf", "guid": "51209", "offsetPos": {"x": 133, "y": 10, "z": 236}, "offsetRotation": {"x": 0, "y": -60, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "8c14", "type": 1, "offsetLoc": {"x": 133, "y": 10, "z": 236}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 18, "dilationRate": 0, "dilationFrame": 0}], "9": [], "10": [], "11": [], "12": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "f861", "breakType": 2}], "14": [], "17": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "de34", "guid": "117541", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0e06", "guid": "153611", "offsetPos": {"x": 0, "y": 0, "z": -85}, "offsetRotation": {"x": -180, "y": 0, "z": -180}, "offsetScale": {"x": 3, "y": 3, "z": 0.05}, "count": -2, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7830", "guid": "153611", "offsetPos": {"x": 0, "y": 0, "z": -85}, "offsetRotation": {"x": -180, "y": 0, "z": -180}, "offsetScale": {"x": 2, "y": 2, "z": 0.05}, "count": -2, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d4bf", "guid": "108249", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -4, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c183", "guid": "108247", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -4, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "6857", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "007b", "guid": "14318", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "4": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "6258", "offsetPos": {"x": 0, "y": 0, "z": 100}, "forceNum": 1500, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "b743", "guid": "162447", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8a3e", "guid": "130643", "offsetPos": {"x": 94, "y": 0, "z": 20}, "offsetRotation": {"x": -45, "y": 0, "z": -90}, "offsetScale": {"x": 3, "y": 3, "z": 1.5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "6": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "6e33", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 8, "xFrequency": 6, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 8, "zFrequency": 6, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2010", "type": 1, "offsetLoc": {"x": 180, "y": 10, "z": 25}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 16, "dilationRate": 0, "dilationFrame": 0}], "7": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "e6d8", "type": 1, "offsetLoc": {"x": 183, "y": 10, "z": 140}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 17, "dilationRate": 0, "dilationFrame": 0}], "8": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "8c14", "type": 1, "offsetLoc": {"x": 133, "y": 10, "z": 236}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 18, "dilationRate": 0, "dilationFrame": 0}], "9": [], "10": [], "11": [], "12": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "f861", "breakType": 2}], "14": [], "17": []}</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "8af7", "guid": "121596", "duration": 28, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "5e76", "offsetPos": {"x": 200, "y": 0, "z": 500}, "forceNum": 1500, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "1": [], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d8fb", "guid": "168955", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": 15, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8fd9", "guid": "168955", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": 16, "colorHex": "", "colorHex1": ""}], "4": [], "5": [], "9": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "886b", "guid": "27702", "offsetPos": {"x": 150, "y": 0, "z": -95}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 15, "y": 15, "z": 15}, "count": 30, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d9d4", "guid": "116457", "offsetPos": {"x": 150, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 18, "y": 18, "z": 18}, "count": 30, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9e88", "guid": "168954", "offsetPos": {"x": 150, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 8, "y": 8, "z": 8}, "count": 30, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "761e", "guid": "146763", "offsetPos": {"x": 150, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 30, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7818", "guid": "51209", "offsetPos": {"x": 150, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 8, "y": 8, "z": 8}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "10": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "df97", "type": 1, "offsetLoc": {"x": 150, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 21, "checkCount": 3, "checkInterval": 1, "keepFrameCount": 30, "rectSocket": -1, "isShake": 0, "cameraShakeId": 0, "effectid": 19, "dilationRate": 0, "dilationFrame": 0}], "12": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "7926", "breakType": 2}], "17": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "8af7", "guid": "121596", "duration": 28, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "5e76", "offsetPos": {"x": 200, "y": 0, "z": 500}, "forceNum": 1500, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "1": [], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d8fb", "guid": "168955", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": 15, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8fd9", "guid": "168955", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": 16, "colorHex": "", "colorHex1": ""}], "4": [], "5": [], "6": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "6aa6", "guid": "205806", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "8": [], "9": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "886b", "guid": "27702", "offsetPos": {"x": 150, "y": 0, "z": -95}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 15, "y": 15, "z": 15}, "count": 30, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d9d4", "guid": "116457", "offsetPos": {"x": 150, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 18, "y": 18, "z": 18}, "count": 30, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9e88", "guid": "168954", "offsetPos": {"x": 150, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 8, "y": 8, "z": 8}, "count": 30, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "761e", "guid": "146763", "offsetPos": {"x": 150, "y": 0, "z": -100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 30, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "10": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "df97", "type": 1, "offsetLoc": {"x": 150, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 21, "checkCount": 3, "checkInterval": 1, "keepFrameCount": 30, "rectSocket": -1, "isShake": 0, "cameraShakeId": 0, "effectid": 19, "dilationRate": 0, "dilationFrame": 0}], "12": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "7926", "breakType": 2}], "17": []}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：update sword skill change
</commit_message>
<xml_diff>
--- a/battleworld/Excel/MotionClip_技能数据.xlsx
+++ b/battleworld/Excel/MotionClip_技能数据.xlsx
@@ -1155,7 +1155,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "6bdb", "guid": "29769", "duration": 12, "animSlot": -1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e1ca", "guid": "145503", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -12, "slotIndex": 17, "colorHex": "", "colorHex1": ""}], "1": [], "2": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "be8a", "guid": "137576", "sound_volume": 1, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "3": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "30b5", "offsetPos": {"x": -1000, "y": 0, "z": 0}, "forceNum": 3000, "groundFriction": 1, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ac13", "guid": "151743", "offsetPos": {"x": 0, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "4": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "23e8", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.4}, {"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "9c5a", "delayTime": 0, "bulletId": 19, "startLoc": {"x": 100, "y": 0, "z": 30}, "endType": 0, "endDis": 2000}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fffb", "guid": "291299", "offsetPos": {"x": 40, "y": 0, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 90}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -9, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "f3ae", "type": 0, "offsetLoc": {"x": 30, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 10, "z": 4}, "range": 1, "checkCount": 3, "checkInterval": 0.1, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 26, "dilationRate": 0, "dilationFrame": 0}], "5": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "476f", "guid": "29769", "pauseCount": 2}], "6": [], "7": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "568f", "breakType": 2}], "8": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "6bdb", "guid": "29769", "duration": 12, "animSlot": -1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e1ca", "guid": "145503", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -12, "slotIndex": 17, "colorHex": "", "colorHex1": ""}], "1": [], "2": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "be8a", "guid": "137576", "sound_volume": 1, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "3": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "30b5", "offsetPos": {"x": -1000, "y": 0, "z": 0}, "forceNum": 3000, "groundFriction": 1, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ac13", "guid": "151743", "offsetPos": {"x": 0, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "4": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "23e8", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.4}, {"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "9c5a", "delayTime": 0, "bulletId": 19, "startLoc": {"x": 100, "y": 0, "z": 30}, "endType": 0, "endDis": 2000}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fffb", "guid": "291299", "offsetPos": {"x": 40, "y": 0, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 90}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -9, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#DDD300FF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "f3ae", "type": 0, "offsetLoc": {"x": 30, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 5, "y": 10, "z": 4}, "range": 1, "checkCount": 3, "checkInterval": 0.1, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 26, "dilationRate": 0, "dilationFrame": 0}], "5": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "476f", "guid": "29769", "pauseCount": 2}], "6": [], "7": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "568f", "breakType": 2}], "8": []}</t>
         </is>
       </c>
     </row>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "b279", "guid": "29723", "duration": 15, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cd37", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -7, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fcbe", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -7, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c629", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -2, "slotIndex": 16, "colorHex": "", "colorHex1": ""}], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8b16", "guid": "151736", "offsetPos": {"x": 500, "y": 10, "z": 20}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 16, "y": 16, "z": 16}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cb67", "guid": "168949", "offsetPos": {"x": 500, "y": 10, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.5, "y": 2.5, "z": 2.5}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "7722", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "735b", "type": 1, "offsetLoc": {"x": 500, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f17e", "guid": "89107", "offsetPos": {"x": 500, "y": 10, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}], "7": [], "8": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4fec", "guid": "168949", "offsetPos": {"x": 1000, "y": 10, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.5, "y": 2.5, "z": 2.5}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9aa7", "guid": "151736", "offsetPos": {"x": 1000, "y": 10, "z": 20}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 16, "y": 16, "z": 16}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "aff5", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "61f2", "type": 1, "offsetLoc": {"x": 1000, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f26b", "guid": "89107", "offsetPos": {"x": 1000, "y": 10, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}], "9": [], "11": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3296", "guid": "168949", "offsetPos": {"x": 1500, "y": 10, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.5, "y": 2.5, "z": 2.5}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d04d", "guid": "151736", "offsetPos": {"x": 1500, "y": 10, "z": 20}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 16, "y": 16, "z": 16}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0077D3FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "d66b", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 6, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 6, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "a395", "type": 1, "offsetLoc": {"x": 1500, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a3b5", "guid": "89107", "offsetPos": {"x": 1500, "y": 10, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}], "12": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "4e15", "breakType": 2}]}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "b279", "guid": "29747", "duration": 10, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cd37", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -7, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#B200FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fcbe", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -7, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#B200FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c629", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -2, "slotIndex": 16, "colorHex": "", "colorHex1": ""}], "1": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "62d7", "guid": "29747", "pauseCount": 1}], "2": [], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a19b", "guid": "295654", "offsetPos": {"x": 500, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "33dd", "type": 1, "offsetLoc": {"x": 500, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "dbb8", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "7ad3", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 20, "xFrequency": 5, "xWaveform": 0, "yAmplitude": 10, "yFrequency": 2, "yWaveform": 1, "zAmplitude": 14, "zFrequency": 7, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}], "4": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fa6f", "guid": "295654", "offsetPos": {"x": 900, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "d7d6", "type": 1, "offsetLoc": {"x": 900, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "716f", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "5": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "735b", "type": 1, "offsetLoc": {"x": 1300, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9b01", "guid": "295654", "offsetPos": {"x": 1300, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "5a34", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e6a2", "guid": "295654", "offsetPos": {"x": 1700, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "44f6", "breakType": 2}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "b99a", "type": 1, "offsetLoc": {"x": 1700, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "3d14", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "7": [], "8": [], "9": [], "11": [], "12": []}</t>
         </is>
       </c>
     </row>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "90fd", "guid": "122510", "duration": 30, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "42ec", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -10, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "88df", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -10, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0c41", "guid": "181010", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.2, "y": 1.2, "z": 1.2}, "count": -10, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#0053FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2dfd", "guid": "168954", "offsetPos": {"x": 0, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 4}, "count": -11, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#6F92B8FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "7f11", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 1}], "5": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "c4f4", "guid": "265134", "sound_volume": 2, "sound_innerRadius": 20000, "sound_maxDistance": 3000}], "7": [], "11": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "d11a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 50, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "20d0", "guid": "89107", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "bcac", "guid": "89107", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d85a", "guid": "168949", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#066EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "19eb", "guid": "135892", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#066EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "02e8", "guid": "130642", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 7, "y": 7, "z": 7}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#066EFFFF"}], "12": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "c5f0", "type": 1, "offsetLoc": {"x": 150, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 11, "checkCount": 5, "checkInterval": 0.1, "keepFrameCount": 5, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 31, "dilationRate": 0, "dilationFrame": 0}], "15": [], "16": [], "18": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "be99", "breakType": 1}]}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "90fd", "guid": "122510", "duration": 30, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "42ec", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -10, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "88df", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -10, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0c41", "guid": "181010", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.2, "y": 1.2, "z": 1.2}, "count": -10, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#0053FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2dfd", "guid": "168954", "offsetPos": {"x": 0, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 4}, "count": -11, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#6F92B8FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "7f11", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 1}], "5": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "c4f4", "guid": "265134", "sound_volume": 2, "sound_innerRadius": 20000, "sound_maxDistance": 3000}], "7": [], "11": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "d11a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 50, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "20d0", "guid": "89107", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "bcac", "guid": "89107", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d85a", "guid": "168949", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#066EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "19eb", "guid": "135892", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#066EFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "02e8", "guid": "130642", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 7, "y": 7, "z": 7}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#066EFFFF"}], "12": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "c5f0", "type": 1, "offsetLoc": {"x": 150, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 11, "checkCount": 5, "checkInterval": 0.1, "keepFrameCount": 5, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 31, "dilationRate": 0, "dilationFrame": 0}], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "7e7a", "breakType": 1}], "15": [], "16": [], "18": []}</t>
         </is>
       </c>
     </row>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "d536", "guid": "85955", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4292", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -10, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8c49", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -10, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "859e", "guid": "168954", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 4}, "count": -10, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#6F92B8FF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "8a78", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "1": [], "2": [], "3": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "faa3", "guid": "85955", "pauseCount": 4}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "c6b9", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.7}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "14f9", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 16, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1c0b", "guid": "163348", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#7687FFFF"}], "7": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "50c6", "guid": "265131", "sound_volume": 1, "sound_innerRadius": 10000, "sound_maxDistance": 3000}], "8": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d713", "guid": "142950", "offsetPos": {"x": -5, "y": 0, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -3, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#0062FFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "ae84", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 2, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 32, "dilationRate": 0, "dilationFrame": 0}], "9": [{"frameNodeType": "MotionFrameNode_Move", "frameGuid": "14d7", "move_offsetPos": {"x": 200, "y": 0, "z": 0}, "move_isFlash": 1, "move_count": 2}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c357", "guid": "168945", "offsetPos": {"x": 100, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 8, "y": 4, "z": 8}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0088FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d26c", "guid": "212729", "offsetPos": {"x": 217, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#007BFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "90d4", "guid": "212729", "offsetPos": {"x": 706, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#007BFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5266", "guid": "212729", "offsetPos": {"x": 1185, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#007BFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fa56", "guid": "212729", "offsetPos": {"x": 1631, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#007BFFFF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "dbe9", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "10": [], "12": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "518d", "guid": "89107", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}], "13": [], "14": [], "15": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "b3fb", "breakType": 2}], "16": [], "17": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "d536", "guid": "279656", "duration": 16, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "8a78", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "1": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d90c", "guid": "158173", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.5, "z": 0.5}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "2": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "b2a2", "guid": "279656", "pauseCount": 1}], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "236a", "guid": "295658", "offsetPos": {"x": 0, "y": 0, "z": -20}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "9f35", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 20, "xFrequency": 0, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 16, "zFrequency": 3, "zWaveform": 1, "fovAmplitude": 100, "fovFrequency": 10, "fovWaveform": 1, "keepTime": 0.5}], "4": [{"frameNodeType": "MotionFrameNode_Move", "frameGuid": "f36b", "move_offsetPos": {"x": 1000, "y": 0, "z": 0}, "move_isFlash": 0, "move_count": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c2cb", "guid": "200145", "offsetPos": {"x": -1400, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 0.7, "z": 0.7}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "9255", "guid": "137559", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "de14", "type": 0, "offsetLoc": {"x": -400, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 15, "y": 4, "z": 4}, "range": 1, "checkCount": 1, "checkInterval": 0.1, "keepFrameCount": 2, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 32, "dilationRate": 0, "dilationFrame": 0}], "6": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "15b4", "breakType": 1}], "7": [], "8": [], "9": [], "10": [], "12": [], "13": [], "14": [], "15": [], "16": [], "17": []}</t>
         </is>
       </c>
     </row>
@@ -1266,11 +1266,11 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "ad79", "guid": "121793", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c608", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 12, "y": 12, "z": 12}, "count": -30, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e9c1", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 12, "y": 12, "z": 12}, "count": -30, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b8e7", "guid": "113913", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 15, "y": 15, "z": 0.1}, "count": -10, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0090FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5ec8", "guid": "113913", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": -55}, "offsetScale": {"x": 15, "y": 15, "z": 0.1}, "count": -10, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#0090FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "60b5", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -7, "slotIndex": 16, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b548", "guid": "163348", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -7, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#7687FFFF"}], "9": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9ad9", "guid": "101412", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.8, "y": 2.8, "z": 2.8}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "dae0", "guid": "192415", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -23, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#0056FFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "bad6", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 16, "checkCount": 3, "checkInterval": 0.1, "keepFrameCount": 3, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 33, "dilationRate": 0, "dilationFrame": 0}], "10": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "d089", "guid": "121793", "pauseCount": 22}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "85d7", "guid": "130743", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "97d9", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b6d7", "guid": "89107", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}], "15": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "15f6", "guid": "101412", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.8, "y": 2.8, "z": 2.8}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "31b4", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 16, "checkCount": 3, "checkInterval": 0.1, "keepFrameCount": 3, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 34, "dilationRate": 0, "dilationFrame": 0}], "16": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b36b", "guid": "130743", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "981c", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9617", "guid": "89107", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}], "18": [], "20": [], "21": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6ff1", "guid": "101412", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.8, "y": 2.8, "z": 2.8}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "8e50", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 16, "checkCount": 3, "checkInterval": 0.1, "keepFrameCount": 3, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 35, "dilationRate": 0, "dilationFrame": 0}], "22": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c57a", "guid": "130743", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "0e78", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5bc4", "guid": "89107", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}], "23": [], "25": [], "26": [], "27": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ba2a", "guid": "101412", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.8, "y": 2.8, "z": 2.8}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "38ec", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 16, "checkCount": 3, "checkInterval": 0.1, "keepFrameCount": 3, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 36, "dilationRate": 0, "dilationFrame": 0}], "28": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b7ef", "guid": "130743", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -8, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "e0cd", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a2ad", "guid": "89107", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}], "30": [], "32": [], "34": [], "36": [], "37": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "d58c", "breakType": 1}], "39": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "ad79", "guid": "285460", "duration": 16, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "aa84", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -6, "slotIndex": 16, "colorHex": "", "colorHex1": ""}], "5": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "2b26", "guid": "285460", "pauseCount": 1}], "6": [], "7": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "de5d", "guid": "295655", "offsetPos": {"x": 240, "y": 40, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color#|AE4448FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d848", "guid": "295655", "offsetPos": {"x": -480, "y": 70, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color#|AE4448FF"}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "70b8", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4e3c", "type": 1, "offsetLoc": {"x": 240, "y": 40, "z": 60}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0.2, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 32, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "35ea", "type": 1, "offsetLoc": {"x": -480, "y": 70, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0.2, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 32, "dilationRate": 0, "dilationFrame": 0}], "8": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7afa", "guid": "295655", "offsetPos": {"x": 60, "y": 320, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#AE4448FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "dfdd", "guid": "295655", "offsetPos": {"x": 120, "y": -480, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#AE4448FF"}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "85b9", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "9f79", "type": 1, "offsetLoc": {"x": 60, "y": 320, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0.2, "keepFrameCount": 1, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 32, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "af0a", "type": 1, "offsetLoc": {"x": 120, "y": -480, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0.2, "keepFrameCount": 1, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 32, "dilationRate": 0, "dilationFrame": 0}], "9": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f2b7", "guid": "295655", "offsetPos": {"x": 590, "y": 430, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#AE4448FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2223", "guid": "295655", "offsetPos": {"x": -670, "y": -410, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#AE4448FF"}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "5988", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "c583", "type": 1, "offsetLoc": {"x": 590, "y": 430, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0.2, "keepFrameCount": 1, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 32, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4e47", "type": 1, "offsetLoc": {"x": -670, "y": -410, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0.2, "keepFrameCount": 1, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 32, "dilationRate": 0, "dilationFrame": 0}], "10": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ecdd", "guid": "295655", "offsetPos": {"x": -420, "y": 370, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1476", "guid": "295655", "offsetPos": {"x": 590, "y": 130, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "d1eb", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2ea1", "type": 1, "offsetLoc": {"x": 590, "y": 370, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0.2, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 32, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "8fe6", "type": 1, "offsetLoc": {"x": -420, "y": 370, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0.2, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 32, "dilationRate": 0, "dilationFrame": 0}], "15": [], "16": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "8418", "breakType": 2}], "18": [], "20": [], "21": [], "22": [], "23": [], "25": [], "26": [], "27": [], "28": []}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：update bullet splash update
</commit_message>
<xml_diff>
--- a/battleworld/Excel/MotionClip_技能数据.xlsx
+++ b/battleworld/Excel/MotionClip_技能数据.xlsx
@@ -833,7 +833,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "62e7", "guid": "20258", "duration": 5, "animSlot": 1}], "2": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "1807", "delayTime": 0, "bulletId": 16, "startLoc": {"x": 135, "y": 55, "z": 50}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3556", "guid": "155715", "offsetPos": {"x": 145, "y": 55, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.8, "y": 0.8, "z": 0.8}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "af8c", "guid": "85156", "offsetPos": {"x": 145, "y": 55, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.7, "y": 0.7, "z": 0.7}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "baa2", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 0.05, "y": 2, "z": 2}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#DEC570FF"}], "3": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "cacb", "breakType": 2}]}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "62e7", "guid": "20258", "duration": 5, "animSlot": 1}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "99fa", "guid": "200780", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "2": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "1807", "delayTime": 0, "bulletId": 16, "startLoc": {"x": 135, "y": 55, "z": 50}, "endType": 0, "endDis": 2500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3556", "guid": "155715", "offsetPos": {"x": 145, "y": 55, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.8, "y": 0.8, "z": 0.8}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "af8c", "guid": "85156", "offsetPos": {"x": 145, "y": 55, "z": 50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.7, "y": 0.7, "z": 0.7}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "baa2", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 0.05, "y": 2, "z": 2}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#DEC570FF"}], "3": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "cacb", "breakType": 2}]}</t>
         </is>
       </c>
     </row>
@@ -856,7 +856,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "a79b", "guid": "156393", "duration": 10, "animSlot": 1}], "2": [], "3": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "7197", "delayTime": 0, "bulletId": 17, "startLoc": {"x": 130, "y": -55, "z": 74}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8289", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "289b", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6eee", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 0.05, "y": 3, "z": 3}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#DEC570FF"}], "4": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "94c5", "breakType": 2}]}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "a79b", "guid": "156393", "duration": 10, "animSlot": 1}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "579e", "guid": "200780", "sound_volume": 1, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "2": [], "3": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "7197", "delayTime": 0, "bulletId": 17, "startLoc": {"x": 130, "y": -55, "z": 74}, "endType": 0, "endDis": 2500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "8289", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "289b", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6eee", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 0.05, "y": 3, "z": 3}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#DEC570FF"}], "4": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "94c5", "breakType": 2}]}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：update magic splash and prefab
</commit_message>
<xml_diff>
--- a/battleworld/Excel/MotionClip_技能数据.xlsx
+++ b/battleworld/Excel/MotionClip_技能数据.xlsx
@@ -1454,7 +1454,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "ab89", "guid": "121964", "duration": 20, "animSlot": 0}], "2": [], "11": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1675", "guid": "142752", "offsetPos": {"x": 400, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 16, "y": 16, "z": 16}, "count": -50, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "7a6a", "type": 1, "offsetLoc": {"x": 400, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 18.56, "checkCount": 20, "checkInterval": 0.2, "keepFrameCount": 40, "rectSocket": -1, "effectid": 53, "dilationRate": 0, "dilationFrame": 0, "cameraShakeId": 0, "isShake": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b561", "guid": "142753", "offsetPos": {"x": 400, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 12, "y": 12, "z": 12}, "count": -50, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFC400FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "e6f8", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "89c2", "breakType": 2}], "16": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "ab89", "guid": "121964", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "161a", "guid": "168958", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -11, "slotIndex": 16, "colorHex": "", "colorHex1": ""}], "2": [], "4": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "998e", "guid": "", "sound_volume": 1, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "10": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d10e", "guid": "89589", "offsetPos": {"x": 250, "y": 0, "z": -120}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "11": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1675", "guid": "142752", "offsetPos": {"x": 400, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 16, "y": 16, "z": 16}, "count": -50, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "7a6a", "type": 1, "offsetLoc": {"x": 400, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 18.56, "checkCount": 20, "checkInterval": 0.2, "keepFrameCount": 40, "rectSocket": -1, "effectid": 53, "dilationRate": 0, "dilationFrame": 0, "cameraShakeId": 0, "isShake": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "b561", "guid": "142753", "offsetPos": {"x": 400, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 12, "y": 12, "z": 12}, "count": -50, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFC400FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "e6f8", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "89c2", "breakType": 2}], "16": []}</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "54e6", "guid": "156393", "duration": 20, "animSlot": 1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "49e1", "guid": "160703", "offsetPos": {"x": 13, "y": 23.32, "z": 80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFBA41FF"}], "1": [], "2": [], "3": [], "4": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "fda1", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "5": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "a89e", "delayTime": 0, "bulletId": 26, "startLoc": {"x": 130, "y": -50, "z": 74}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "40cd", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "982c", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "7f44", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "6": [], "7": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "b53c", "delayTime": 0, "bulletId": 26, "startLoc": {"x": 130, "y": -50, "z": 74}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "06c3", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d8e9", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "100f", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "8": [], "9": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "8c13", "delayTime": 0, "bulletId": 26, "startLoc": {"x": 130, "y": -50, "z": 74}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "06b1", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2513", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "09bd", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "10": [], "11": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "0c17", "delayTime": 0, "bulletId": 26, "startLoc": {"x": 130, "y": -50, "z": 74}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a2f3", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cb00", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "1e6e", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "547b", "breakType": 2}]}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "54e6", "guid": "156393", "duration": 20, "animSlot": 1}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "49e1", "guid": "160703", "offsetPos": {"x": 13, "y": 23.32, "z": 80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -5, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFBA41FF"}], "1": [], "2": [], "3": [], "4": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "fda1", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "5": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "a89e", "delayTime": 0, "bulletId": 26, "startLoc": {"x": 130, "y": -50, "z": 74}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "40cd", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "982c", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "7f44", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "6": [{"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "d85f", "guid": "162446", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "7": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "b53c", "delayTime": 0, "bulletId": 26, "startLoc": {"x": 130, "y": -50, "z": 74}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "06c3", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d8e9", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "100f", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "8": [{"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "bf17", "guid": "162446", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "9": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "8c13", "delayTime": 0, "bulletId": 26, "startLoc": {"x": 130, "y": -50, "z": 74}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "06b1", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2513", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "09bd", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "10": [{"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "30a8", "guid": "162446", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "11": [{"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "0c17", "delayTime": 0, "bulletId": 26, "startLoc": {"x": 130, "y": -50, "z": 74}, "endType": 0, "endDis": 1500}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a2f3", "guid": "155715", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cb00", "guid": "85156", "offsetPos": {"x": 140, "y": -50, "z": 74}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "1e6e", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "547b", "breakType": 2}]}</t>
         </is>
       </c>
     </row>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "7871", "guid": "156436", "duration": 20, "animSlot": 0}], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4284", "guid": "160703", "offsetPos": {"x": 14.1, "y": 20.24, "z": 81.01}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -3, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFE85DFF"}], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f84a", "guid": "155715", "offsetPos": {"x": 210, "y": -50, "z": 30}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "63d3", "guid": "85156", "offsetPos": {"x": 210, "y": -50, "z": 30}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3aca", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 0.05, "y": 4, "z": 4}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#DEC570FF"}, {"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "4f56", "delayTime": 0, "bulletId": 27, "startLoc": {"x": 210, "y": -50, "z": 80}, "endType": 0, "endDis": 3000}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "f4df", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "10": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "205b", "breakType": 1}]}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "7871", "guid": "156436", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cc20", "guid": "160703", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -6, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFE85DFF"}], "3": [], "5": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "22ae", "guid": "162451", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f84a", "guid": "155715", "offsetPos": {"x": 210, "y": -50, "z": 30}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "63d3", "guid": "85156", "offsetPos": {"x": 210, "y": -50, "z": 30}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFCC00FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3aca", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 0.05, "y": 4, "z": 4}, "count": -3, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#DEC570FF"}, {"frameNodeType": "MotionFrameNode_FlyEntity", "frameGuid": "4f56", "delayTime": 0, "bulletId": 27, "startLoc": {"x": 210, "y": -50, "z": 80}, "endType": 0, "endDis": 3000}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "f4df", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9c77", "guid": "137835", "offsetPos": {"x": 150, "y": 0, "z": 60}, "offsetRotation": {"x": 0, "y": 0, "z": -90}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFA4EFF"}], "10": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "205b", "breakType": 1}]}</t>
         </is>
       </c>
     </row>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "0c10", "guid": "117344", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c5a7", "guid": "172886", "offsetPos": {"x": 14, "y": 20, "z": 81}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -15, "slotIndex": 16, "colorHex": "#FFC80000", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "08b2", "guid": "113922", "offsetPos": {"x": -6.71, "y": 0, "z": -18.7}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -10, "slotIndex": 12, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4796", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "10": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e475", "guid": "92839", "offsetPos": {"x": 50, "y": 0, "z": 40}, "offsetRotation": {"x": 0, "y": 5, "z": 0}, "offsetScale": {"x": 4, "y": 6, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFD04CFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2c40", "guid": "92839", "offsetPos": {"x": 50, "y": 0, "z": 40}, "offsetRotation": {"x": 0, "y": 5, "z": -35}, "offsetScale": {"x": 4, "y": 6, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFD04CFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "1c3e", "guid": "92839", "offsetPos": {"x": 50, "y": 0, "z": 40}, "offsetRotation": {"x": 0, "y": 5, "z": 35}, "offsetScale": {"x": 4, "y": 6, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFD04CFF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "9550", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "11": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3c31", "guid": "154053", "offsetPos": {"x": 500, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 2, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFB900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3a8b", "guid": "154053", "offsetPos": {"x": 500, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": 2, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFB900FF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2665", "type": 1, "offsetLoc": {"x": 500, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 17, "checkCount": 25, "checkInterval": 0.2, "keepFrameCount": 50, "rectSocket": -1, "isShake": 0, "cameraShakeId": 0, "effectid": 56, "dilationRate": 0, "dilationFrame": 0}], "12": [], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "bbe7", "breakType": 2}], "33": [], "35": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "0c10", "guid": "117344", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c5a7", "guid": "172886", "offsetPos": {"x": 14, "y": 20, "z": 81}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 4, "y": 4, "z": 4}, "count": -15, "slotIndex": 16, "colorHex": "#FFC80000", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "08b2", "guid": "113922", "offsetPos": {"x": -6.71, "y": 0, "z": -18.7}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -10, "slotIndex": 12, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4796", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}], "10": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e475", "guid": "271321", "offsetPos": {"x": 500, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 5, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -20, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFD04CFF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "9550", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "11": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3c31", "guid": "152589", "offsetPos": {"x": 500, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FE3F3FFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2665", "type": 1, "offsetLoc": {"x": 500, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 17, "checkCount": 25, "checkInterval": 0.2, "keepFrameCount": 25, "rectSocket": -1, "isShake": 0, "cameraShakeId": 0, "effectid": 56, "dilationRate": 0, "dilationFrame": 0}], "12": [], "14": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "bbe7", "breakType": 2}], "30": [], "33": [], "35": []}</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "e6f0", "guid": "121802", "duration": 22, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2603", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "add9", "guid": "168955", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -8, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFA900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6db4", "guid": "168955", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -8, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFA900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "090e", "guid": "146785", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -8, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFA900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5cc2", "guid": "146785", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -8, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFA900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4403", "guid": "78470", "offsetPos": {"x": 100, "y": 0, "z": 30}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "1": [], "8": [], "9": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "f49f", "offsetPos": {"x": -100, "y": 0, "z": 0}, "forceNum": 1000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "9c84", "type": 0, "offsetLoc": {"x": 1382, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 27.8, "y": 2.5, "z": 2.5}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 57, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "cf5f", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "11": [], "13": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "19e4", "breakType": 2}]}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "e6f0", "guid": "121802", "duration": 22, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "2603", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 46, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "add9", "guid": "168955", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -8, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFA900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6db4", "guid": "168955", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -8, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFA900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "090e", "guid": "146785", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -8, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFA900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5cc2", "guid": "146785", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -8, "slotIndex": 16, "colorHex": "", "colorHex1": "Color|#FFA900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4403", "guid": "78470", "offsetPos": {"x": 100, "y": 0, "z": 30}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 0.5, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "1": [], "8": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "f9c9", "guid": "162452", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "9": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "f49f", "offsetPos": {"x": -100, "y": 0, "z": 0}, "forceNum": 1000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "9c84", "type": 0, "offsetLoc": {"x": 1382, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 27.8, "y": 2.5, "z": 2.5}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 57, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "cf5f", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 4, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 4, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "11": [], "13": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "19e4", "breakType": 2}]}</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "2f55", "guid": "121902", "duration": 20, "animSlot": 1}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "db1f", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 47, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3e0e", "guid": "106127", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -14, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFA900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c8e6", "guid": "146785", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -14, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFA900FF"}], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "935f", "guid": "144095", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0f51", "guid": "144090", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "7": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "7e31", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 58, "dilationRate": 0, "dilationFrame": 0}], "9": [], "17": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "9ce1", "breakType": 2}], "19": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "2f55", "guid": "121902", "duration": 20, "animSlot": 1}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "db1f", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 47, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3e0e", "guid": "106127", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -14, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFA900FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c8e6", "guid": "146785", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -14, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFA900FF"}], "5": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "7280", "guid": "307720", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "935f", "guid": "144095", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0f51", "guid": "144090", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "7": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "7e31", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 58, "dilationRate": 0, "dilationFrame": 0}], "9": [], "17": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "9ce1", "breakType": 2}], "19": []}</t>
         </is>
       </c>
     </row>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "56f6", "guid": "121793", "duration": 15, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3728", "guid": "89075", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6d97", "guid": "142750", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -9, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cc76", "guid": "144090", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "f9ab", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 59, "dilationRate": 0, "dilationFrame": 0}], "8": [], "9": [], "10": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "c02b", "breakType": 2}]}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "56f6", "guid": "121793", "duration": 15, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "3728", "guid": "89075", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "4": [{"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "380d", "guid": "307720", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6d97", "guid": "142750", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": -9, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cc76", "guid": "144090", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "f9ab", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 59, "dilationRate": 0, "dilationFrame": 0}], "8": [], "9": [], "10": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "c02b", "breakType": 2}]}</t>
         </is>
       </c>
     </row>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "ef4d", "guid": "84913", "duration": 18, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "241a", "guid": "88801", "offsetPos": {"x": 0, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.6, "y": 2.6, "z": 2.6}, "count": -4, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "cc09", "offsetPos": {"x": 0, "y": 0, "z": -1500}, "forceNum": 3000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "4": [], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a88f", "guid": "135888", "offsetPos": {"x": 0, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "00FFE900", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d693", "guid": "151574", "offsetPos": {"x": 0, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 20, "y": 20, "z": 20}, "count": 1, "slotIndex": -1, "colorHex": "000000", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "f305", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 25, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 60, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "338d", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}], "7": [], "8": [], "10": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "2374", "breakType": 2}], "12": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "ef4d", "guid": "84913", "duration": 18, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "241a", "guid": "88801", "offsetPos": {"x": 0, "y": 0, "z": 100}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2.6, "y": 2.6, "z": 2.6}, "count": -4, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "cc09", "offsetPos": {"x": 0, "y": 0, "z": -1500}, "forceNum": 3000, "groundFriction": 2, "gravityScale": 1, "gravityTime": 0}], "4": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "ed4b", "guid": "206042", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "5": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a88f", "guid": "135888", "offsetPos": {"x": 0, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "00FFE900", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "d693", "guid": "151574", "offsetPos": {"x": 0, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 20, "y": 20, "z": 20}, "count": 1, "slotIndex": -1, "colorHex": "000000", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "f305", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 25, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 60, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "338d", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}], "7": [], "8": [], "10": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "2374", "breakType": 2}], "12": []}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：update final anim data change
</commit_message>
<xml_diff>
--- a/battleworld/Excel/MotionClip_技能数据.xlsx
+++ b/battleworld/Excel/MotionClip_技能数据.xlsx
@@ -1017,7 +1017,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "9ca6", "guid": "121603", "duration": 15, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "40cb", "guid": "142755", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -13, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "def6", "guid": "142755", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -13, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a8f3", "guid": "162430", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -13, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "8": [], "9": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0646", "guid": "158124", "offsetPos": {"x": 0, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9be4", "guid": "181022", "offsetPos": {"x": 0, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0f3b", "guid": "27702", "offsetPos": {"x": 0, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4378", "guid": "51209", "offsetPos": {"x": 0, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4ef7", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 2}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 13, "dilationRate": 0, "dilationFrame": 0}], "10": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "b0f3", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 14, "dilationRate": 0, "dilationFrame": 0}], "11": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "af5e", "breakType": 2}], "13": [], "14": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "9ca6", "guid": "121603", "duration": 15, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "40cb", "guid": "142755", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -13, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "def6", "guid": "142755", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -13, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "4": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "165a", "guid": "200876", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "5": [], "7": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "300c", "guid": "298312", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c6cc", "guid": "142961", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "44f7", "guid": "89129", "offsetPos": {"x": 0, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "8": [], "9": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4ef7", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 2}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 13, "dilationRate": 0, "dilationFrame": 0}], "10": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "b0f3", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": -100}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 6, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 14, "dilationRate": 0, "dilationFrame": 0}], "11": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "af5e", "breakType": 2}], "13": [], "14": []}</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "10db", "guid": "122492", "duration": 15, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "66c1", "guid": "88441", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.2, "y": 1.2, "z": 1.2}, "count": -6, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "1": [], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a6c5", "guid": "168944", "offsetPos": {"x": 5, "y": 4, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": 15, "colorHex": "", "colorHex1": ""}], "4": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4dd1", "guid": "153044", "offsetPos": {"x": 8, "y": -25, "z": 101}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "497b", "guid": "151577", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 12, "y": 12, "z": 0.2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "fe17", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 20, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4329", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 21, "dilationRate": 0, "dilationFrame": 0}], "5": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "f5cb", "breakType": 2}], "6": [], "7": [], "10": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "10db", "guid": "122492", "duration": 15, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "66c1", "guid": "88441", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.2, "y": 1.2, "z": 1.2}, "count": -6, "slotIndex": 15, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}], "1": [], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a6c5", "guid": "168944", "offsetPos": {"x": 5, "y": 4, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": 15, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "1e28", "guid": "205238", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "4": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4dd1", "guid": "153044", "offsetPos": {"x": 8, "y": -25, "z": 300}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 10, "y": 10, "z": 10}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "497b", "guid": "151577", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 12, "y": 12, "z": 0.2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FFFFFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "fe17", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 20, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "4329", "type": 1, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 21, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "125b", "guid": "130642", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "5": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "f5cb", "breakType": 2}], "6": [], "7": [], "10": []}</t>
         </is>
       </c>
     </row>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "b279", "guid": "29747", "duration": 10, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cd37", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -7, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#B200FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fcbe", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -7, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#B200FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c629", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -2, "slotIndex": 16, "colorHex": "", "colorHex1": ""}], "1": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "62d7", "guid": "29747", "pauseCount": 1}], "2": [], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a19b", "guid": "295654", "offsetPos": {"x": 500, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "33dd", "type": 1, "offsetLoc": {"x": 500, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "dbb8", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "7ad3", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 20, "xFrequency": 5, "xWaveform": 0, "yAmplitude": 10, "yFrequency": 2, "yWaveform": 1, "zAmplitude": 14, "zFrequency": 7, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}], "4": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fa6f", "guid": "295654", "offsetPos": {"x": 900, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "d7d6", "type": 1, "offsetLoc": {"x": 900, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "716f", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "5": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "735b", "type": 1, "offsetLoc": {"x": 1300, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9b01", "guid": "295654", "offsetPos": {"x": 1300, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "5a34", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e6a2", "guid": "295654", "offsetPos": {"x": 1700, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "44f6", "breakType": 2}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "b99a", "type": 1, "offsetLoc": {"x": 1700, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "3d14", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "7": [], "8": [], "9": [], "11": [], "12": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "b279", "guid": "29747", "duration": 10, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cd37", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -7, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#B200FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fcbe", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -7, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#B200FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "c629", "guid": "163346", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -2, "slotIndex": 16, "colorHex": "", "colorHex1": ""}], "1": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "62d7", "guid": "29747", "pauseCount": 1}], "2": [], "3": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a19b", "guid": "295654", "offsetPos": {"x": 500, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "33dd", "type": 1, "offsetLoc": {"x": 500, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "dbb8", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "7ad3", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 20, "xFrequency": 5, "xWaveform": 0, "yAmplitude": 10, "yFrequency": 2, "yWaveform": 1, "zAmplitude": 14, "zFrequency": 7, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.2}], "4": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fa6f", "guid": "295654", "offsetPos": {"x": 900, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "d7d6", "type": 1, "offsetLoc": {"x": 900, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "716f", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "5": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "735b", "type": 1, "offsetLoc": {"x": 1300, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9b01", "guid": "295654", "offsetPos": {"x": 1300, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "5a34", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e6a2", "guid": "295654", "offsetPos": {"x": 1700, "y": 0, "z": -80}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "44f6", "breakType": 2}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "b99a", "type": 1, "offsetLoc": {"x": 1700, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 10, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 27, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "3d14", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "7": [], "8": [], "9": [], "11": [], "12": []}</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "31bd", "guid": "162135", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "32c3", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -6, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a346", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -6, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#0089FFFF"}], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cee1", "guid": "89107", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "87d8", "guid": "151577", "offsetPos": {"x": 0, "y": 0, "z": 120}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -5, "slotIndex": 23, "colorHex": "#FF000000", "colorHex1": "Color|#006EFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "70c2", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 40, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ad46", "guid": "168949", "offsetPos": {"x": 0, "y": 0, "z": -10}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0d3a", "guid": "89107", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "febe", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "8": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "ff73", "breakType": 2}], "9": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "31bd", "guid": "162135", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "32c3", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -6, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a346", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": -6, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#0089FFFF"}], "5": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "cffb", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "cee1", "guid": "89107", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "87d8", "guid": "151577", "offsetPos": {"x": 0, "y": 0, "z": 120}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -5, "slotIndex": 23, "colorHex": "#FF000000", "colorHex1": "Color|#006EFFFF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "70c2", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 40, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "ad46", "guid": "168949", "offsetPos": {"x": 0, "y": 0, "z": -10}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0d3a", "guid": "89107", "offsetPos": {"x": 0, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1, "y": 1, "z": 1}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "febe", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "8": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "ff73", "breakType": 2}], "9": []}</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "8437", "guid": "85120", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fa60", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -9, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f76a", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -9, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5291", "guid": "168954", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 7, "y": 7, "z": 7}, "count": -7, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#6F92B8FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "121e", "guid": "13711", "offsetPos": {"x": 150, "y": 0, "z": 120}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -7, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#6F92B8FF"}], "7": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f5fe", "guid": "295658", "offsetPos": {"x": 150, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 7, "y": 7, "z": 7}, "count": -7, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "913c", "guid": "168949", "offsetPos": {"x": 150, "y": 0, "z": -10}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "cd70", "type": 1, "offsetLoc": {"x": 150, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 25, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 41, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "cbfe", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "9": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "61bf", "guid": "89107", "offsetPos": {"x": 150, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}], "10": [], "11": [], "12": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "0168", "breakType": 2}], "13": [], "14": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "8437", "guid": "85120", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fa60", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -9, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f76a", "guid": "27694", "offsetPos": {"x": 0, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": -9, "slotIndex": 12, "colorHex": "", "colorHex1": "Color|#0089FFFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5291", "guid": "168954", "offsetPos": {"x": 150, "y": 0, "z": -70}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 7, "y": 7, "z": 7}, "count": -7, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#6F92B8FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "121e", "guid": "13711", "offsetPos": {"x": 150, "y": 0, "z": 120}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -7, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#6F92B8FF"}], "6": [{"frameNodeType": "MotionFrameNode_Sound", "frameGuid": "7227", "guid": "137576", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000}], "7": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "f5fe", "guid": "295658", "offsetPos": {"x": 150, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 7, "y": 7, "z": 7}, "count": -7, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "913c", "guid": "168949", "offsetPos": {"x": 150, "y": 0, "z": -30}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "cd70", "type": 1, "offsetLoc": {"x": 150, "y": 0, "z": -80}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 25, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 41, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "cbfe", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 4, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 4, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}], "9": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "61bf", "guid": "89107", "offsetPos": {"x": 150, "y": 0, "z": -60}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": -6, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#009BFFFF"}], "10": [], "11": [], "12": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "0168", "breakType": 2}], "13": [], "14": []}</t>
         </is>
       </c>
     </row>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "ee5b", "guid": "279750", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "c323", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 47, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0e01", "guid": "151574", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9516", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -180}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 7, "y": 7, "z": 7}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "1": [], "4": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "feb3", "guid": "105195", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 50}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "#Color|#FF004DFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6187", "guid": "31118", "offsetPos": {"x": 40, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 50}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "#Color|#FF004DFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2ee5", "guid": "31118", "offsetPos": {"x": 40, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 30}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "#Color|#FF004DFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "aa4b", "guid": "31118", "offsetPos": {"x": 40, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 50}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "#Color|#FF004DFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5d92", "guid": "31118", "offsetPos": {"x": 40, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 30}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "#Color|#FF004DFF"}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "15d2", "guid": "298500", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "5": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "ed71", "offsetPos": {"x": 300, "y": 0, "z": 0}, "forceNum": 750, "groundFriction": 0, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "159a", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 6, "y": 6, "z": 6}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 62, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "f44e", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 6, "y": 6, "z": 6}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 62, "dilationRate": 0, "dilationFrame": 0}], "6": [], "7": [], "8": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e9ee", "guid": "105195", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 250}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2c72", "guid": "31118", "offsetPos": {"x": 30, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 250}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fef3", "guid": "31118", "offsetPos": {"x": 30, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 230}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7acc", "guid": "31118", "offsetPos": {"x": 30, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 250}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e181", "guid": "31118", "offsetPos": {"x": 30, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 230}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "8666", "guid": "298496", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "9": [], "10": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "5c44", "guid": "279750", "pauseCount": 1}], "11": [], "12": [], "13": [], "15": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "c46e", "breakType": 2}], "16": [], "17": [], "18": [], "19": [], "20": [], "21": [], "22": [], "23": [], "25": [], "27": [], "30": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "ee5b", "guid": "279750", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "c323", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 47, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0e01", "guid": "151574", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": -5, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "9516", "guid": "145518", "offsetPos": {"x": 0, "y": 0, "z": -180}, "offsetRotation": {"x": 0, "y": -90, "z": 0}, "offsetScale": {"x": 7, "y": 7, "z": 7}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "1": [], "4": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "feb3", "guid": "105195", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 50}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "#Color|#FF004DFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "6187", "guid": "31118", "offsetPos": {"x": 40, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 50}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "#Color|#FF004DFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2ee5", "guid": "31118", "offsetPos": {"x": 40, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 30}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "#Color|#FF004DFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "aa4b", "guid": "31118", "offsetPos": {"x": 40, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 50}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "#Color|#FF004DFF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5d92", "guid": "31118", "offsetPos": {"x": 40, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 30}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "#Color|#FF004DFF"}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "15d2", "guid": "298500", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "5": [{"frameNodeType": "MotionFrameNode_impulse", "frameGuid": "ed71", "offsetPos": {"x": 300, "y": 0, "z": 0}, "forceNum": 750, "groundFriction": 0, "gravityScale": 1, "gravityTime": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "159a", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 6, "y": 6, "z": 6}, "range": 1, "checkCount": 1, "checkInterval": 0.4, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 62, "dilationRate": 0, "dilationFrame": 0}], "6": [], "7": [], "8": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e9ee", "guid": "105195", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 250}, "offsetScale": {"x": 3, "y": 3, "z": 3}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "2c72", "guid": "31118", "offsetPos": {"x": 30, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 250}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "fef3", "guid": "31118", "offsetPos": {"x": 30, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 230}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "7acc", "guid": "31118", "offsetPos": {"x": 30, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 250}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "e181", "guid": "31118", "offsetPos": {"x": 30, "y": 0, "z": -50}, "offsetRotation": {"x": 0, "y": 0, "z": 230}, "offsetScale": {"x": 5, "y": 5, "z": 5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_3DSound", "frameGuid": "8666", "guid": "298496", "sound_volume": 10, "sound_innerRadius": 100, "sound_maxDistance": 3000, "sound_count": 0, "bind": 1}], "9": [{"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "5ec9", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 6, "y": 6, "z": 6}, "range": 1, "checkCount": 0.4, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 62, "dilationRate": 0, "dilationFrame": 0}], "10": [{"frameNodeType": "MotionFrameNode_AnimPause", "frameGuid": "5c44", "guid": "279750", "pauseCount": 1}], "11": [], "12": [], "13": [], "15": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "c46e", "breakType": 2}], "16": [], "17": [], "18": [], "19": [], "20": [], "21": [], "22": [], "23": [], "25": [], "27": [], "30": []}</t>
         </is>
       </c>
     </row>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "dfd1", "guid": "121793", "duration": 14, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0d75", "guid": "162217", "offsetPos": {"x": 4.61, "y": 2.26, "z": 0.72}, "offsetRotation": {"x": -5.33, "y": -14.76, "z": 0.91}, "offsetScale": {"x": 3, "y": 3, "z": 2.1}, "count": -15, "slotIndex": 16, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a981", "guid": "162431", "offsetPos": {"x": 30, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF4300FF"}], "2": [], "3": [], "4": [], "5": [], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4e14", "guid": "158124", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FF3700FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "781a", "guid": "144090", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FF3700FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "672b", "guid": "95651", "offsetPos": {"x": 0, "y": 0, "z": -120}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3700FF"}], "7": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "9a9a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 6, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 6, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "ee63", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 78, "dilationRate": 0, "dilationFrame": 0}], "8": [], "9": [], "11": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "ab5b", "breakType": 2}], "15": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "dfd1", "guid": "121793", "duration": 14, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "0d75", "guid": "162217", "offsetPos": {"x": 4.61, "y": 2.26, "z": 0.72}, "offsetRotation": {"x": -5.33, "y": -14.76, "z": 0.91}, "offsetScale": {"x": 3, "y": 3, "z": 2.1}, "count": -15, "slotIndex": 16, "colorHex": "", "colorHex1": ""}], "2": [], "3": [], "4": [], "5": [], "6": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "4e14", "guid": "158124", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FF3700FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "781a", "guid": "144090", "offsetPos": {"x": 0, "y": 0, "z": 0}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 2}, "count": 1, "slotIndex": 23, "colorHex": "", "colorHex1": "Color|#FF3700FF"}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "672b", "guid": "95651", "offsetPos": {"x": 0, "y": 0, "z": -120}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 3, "y": 3, "z": 4}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF3700FF"}], "7": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "9a9a", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 2, "xFrequency": 6, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 2, "zFrequency": 6, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.3}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "ee63", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 78, "dilationRate": 0, "dilationFrame": 0}], "8": [], "9": [], "11": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "ab5b", "breakType": 2}], "15": []}</t>
         </is>
       </c>
     </row>
@@ -1910,11 +1910,11 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "c7b4", "guid": "121905", "duration": 20, "animSlot": 0}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "347d", "guid": "162431", "offsetPos": {"x": 30, "y": 0, "z": -90}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 2, "y": 2, "z": 1}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF4300FF"}], "2": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a600", "guid": "163348", "offsetPos": {"x": 75, "y": 0, "z": 42}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "16a8", "guid": "163348", "offsetPos": {"x": 75, "y": 0, "z": 42}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "3": [], "4": [], "5": [], "9": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "0f88", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5095", "guid": "151573", "offsetPos": {"x": 75, "y": 0, "z": 42}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF6A00FF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "37c9", "type": 1, "offsetLoc": {"x": 75, "y": 0, "z": -38}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 80, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "08a3", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 79, "dilationRate": 0, "dilationFrame": 0}], "12": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "3109", "breakType": 2}], "13": [], "16": []}</t>
+          <t>{"0": [{"frameNodeType": "MotionFrameNode_Animation", "frameGuid": "c7b4", "guid": "121905", "duration": 20, "animSlot": 0}], "2": [{"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "a600", "guid": "163348", "offsetPos": {"x": 75, "y": 0, "z": 42}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "16a8", "guid": "163348", "offsetPos": {"x": 75, "y": 0, "z": 42}, "offsetRotation": {"x": 0, "y": 90, "z": 0}, "offsetScale": {"x": 1.5, "y": 1.5, "z": 1.5}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": ""}], "3": [], "4": [], "5": [], "9": [{"frameNodeType": "MotionFrameNode_Shake", "frameGuid": "0f88", "rollAmplitude": 0, "rollFrequency": 0, "rollWaveform": 1, "pitchAmplitude": 0, "pitchFrequency": 0, "pitchWaveform": 1, "yawAmplitude": 0, "yawFrequency": 0, "yawWaveform": 1, "xAmplitude": 10, "xFrequency": 10, "xWaveform": 1, "yAmplitude": 0, "yFrequency": 0, "yWaveform": 1, "zAmplitude": 10, "zFrequency": 10, "zWaveform": 1, "fovAmplitude": 0, "fovFrequency": 0, "fovWaveform": 1, "keepTime": 0.5}, {"frameNodeType": "MotionFrameNode_Effect", "frameGuid": "5095", "guid": "151573", "offsetPos": {"x": 75, "y": 0, "z": 42}, "offsetRotation": {"x": 0, "y": 0, "z": 0}, "offsetScale": {"x": 6, "y": 6, "z": 6}, "count": 1, "slotIndex": -1, "colorHex": "", "colorHex1": "Color|#FF6A00FF"}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "37c9", "type": 1, "offsetLoc": {"x": 75, "y": 0, "z": -38}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 5, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 80, "dilationRate": 0, "dilationFrame": 0}, {"frameNodeType": "MotionFrameNode_SkillRect", "frameGuid": "08a3", "type": 0, "offsetLoc": {"x": 0, "y": 0, "z": 0}, "offsetRot": {"x": 0, "y": 0, "z": 0}, "LWH": {"x": 1, "y": 1, "z": 1}, "range": 1, "checkCount": 1, "checkInterval": 0, "keepFrameCount": 0, "rectSocket": 0, "isShake": 0, "cameraShakeId": 0, "effectid": 79, "dilationRate": 0, "dilationFrame": 0}], "12": [{"frameNodeType": "MotionFrameNode_BreakPoint", "frameGuid": "3109", "breakType": 2}], "13": [], "16": []}</t>
         </is>
       </c>
     </row>

</xml_diff>